<commit_message>
Properly showing animating objects with different rows/cols
Fixed not properly shown some of the monsters who has different row/cols in their animation frames.
Minor refactoring: changed all of the members in the GameObject class to start with the "m_" prefix.
Fixed properly animating objects going row after row (before was going column after column)
</commit_message>
<xml_diff>
--- a/calcs.xlsx
+++ b/calcs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8136" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8136"/>
   </bookViews>
   <sheets>
     <sheet name="frames" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="zero movement" sheetId="5" r:id="rId4"/>
     <sheet name="colide" sheetId="6" r:id="rId5"/>
     <sheet name="process wall colision" sheetId="7" r:id="rId6"/>
+    <sheet name="scaleSpriteTo" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="117">
   <si>
     <t>y \ x</t>
   </si>
@@ -472,12 +473,54 @@
   <si>
     <t>O2</t>
   </si>
+  <si>
+    <t>w * m_frames.framesAlongX / texture.getSize().x;</t>
+  </si>
+  <si>
+    <t>h * m_frames.framesAlongY / texture.getSize().y;</t>
+  </si>
+  <si>
+    <t>m_frames.framesAlongX</t>
+  </si>
+  <si>
+    <t>m_frames.framesAlongY</t>
+  </si>
+  <si>
+    <t>textureSizeX</t>
+  </si>
+  <si>
+    <t>textureSizeY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            int width = texture.Width / columnsForAnimation;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            int height = texture.Height / rowsForAnimation;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            int row = (int)((float)currentFrame / (float)columnsForAnimation);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            int column = currentFrame % columnsForAnimation;</t>
+  </si>
+  <si>
+    <t>texture.Width / columnsForAnimation;</t>
+  </si>
+  <si>
+    <t>texture.Height / rowsForAnimation;</t>
+  </si>
+  <si>
+    <t>row</t>
+  </si>
+  <si>
+    <t>column</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -513,8 +556,15 @@
       <family val="3"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -560,6 +610,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -671,16 +727,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -715,6 +765,22 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -860,11 +926,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="133463040"/>
-        <c:axId val="133513984"/>
+        <c:axId val="293212544"/>
+        <c:axId val="293214080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="133463040"/>
+        <c:axId val="293212544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="800"/>
@@ -875,13 +941,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133513984"/>
+        <c:crossAx val="293214080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133513984"/>
+        <c:axId val="293214080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -892,7 +958,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133463040"/>
+        <c:crossAx val="293212544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1880,7 +1946,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1888,194 +1954,378 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E17"/>
+  <dimension ref="A2:Q23"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="8.88671875" style="27"/>
+    <col min="9" max="9" width="12.109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="27"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="26">
         <f>$B12*B3</f>
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="26">
         <f t="shared" ref="C2:E2" si="0">$B12*C3</f>
         <v>75</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="26">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="26">
         <f t="shared" si="0"/>
         <v>225</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="F2" s="27">
+        <v>300</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="26">
+        <f>$B12*J3</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="26">
+        <v>100</v>
+      </c>
+      <c r="L2" s="26">
+        <v>200</v>
+      </c>
+      <c r="M2" s="26">
+        <v>300</v>
+      </c>
+      <c r="N2" s="26">
+        <v>400</v>
+      </c>
+      <c r="O2" s="26">
+        <v>500</v>
+      </c>
+      <c r="P2" s="26">
+        <v>600</v>
+      </c>
+      <c r="Q2" s="26">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="28">
         <f>B$13*0</f>
         <v>0</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="29">
         <v>0</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="29">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="29">
         <v>2</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="29">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="I3" s="28">
+        <f>J$13*0</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="29">
+        <v>0</v>
+      </c>
+      <c r="K3" s="29">
+        <v>1</v>
+      </c>
+      <c r="L3" s="29">
+        <v>2</v>
+      </c>
+      <c r="M3" s="29">
+        <v>3</v>
+      </c>
+      <c r="N3" s="29">
+        <v>4</v>
+      </c>
+      <c r="O3" s="29">
+        <v>5</v>
+      </c>
+      <c r="P3" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="28">
         <f>B$13*1</f>
         <v>50</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="29">
         <v>4</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="29">
         <v>5</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="29">
         <v>6</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="29">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="I4" s="28">
+        <v>100</v>
+      </c>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+    </row>
+    <row r="5" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="28">
         <f>B$13*2</f>
         <v>100</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="29">
         <v>8</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="29">
         <v>9</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="29">
         <v>10</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="29">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+    </row>
+    <row r="6" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="28">
         <f>B$13*3</f>
         <v>150</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="29">
         <v>12</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="29">
         <v>13</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="29">
         <v>14</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="29">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="27">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="30">
         <v>300</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="I8" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="30">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="30">
         <v>200</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="I9" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="30">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="I10" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="30">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="I11" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="27">
         <f>B8/B10</f>
         <v>75</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="I12" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" s="27">
+        <f>J8/J10</f>
+        <v>100</v>
+      </c>
+      <c r="K12" s="27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="27">
         <f>B9/B11</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="I13" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="27">
+        <f>J9/J11</f>
+        <v>100</v>
+      </c>
+      <c r="K13" s="27" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="27">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="I15" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="27">
         <f>MOD(B15,B10) *B12</f>
         <v>150</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="27" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="I16" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="27">
+        <f>MOD(J15,J10) *J12</f>
+        <v>100</v>
+      </c>
+      <c r="K16" s="27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="27">
         <f>ROUNDDOWN(B15/B10,0) *B13</f>
         <v>100</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="27" t="s">
         <v>11</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="27">
+        <f>ROUNDDOWN(J15/J10,0) *J13</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I18" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="J18" s="27">
+        <f>ROUNDDOWN(J15/J10, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I19" s="27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="27" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2242,124 +2492,124 @@
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="4"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="4"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="4"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="4"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="4"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="2"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="4"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="2"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
@@ -2386,7 +2636,7 @@
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C20">
@@ -2398,7 +2648,7 @@
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C21">
@@ -2418,7 +2668,7 @@
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C24">
@@ -2430,7 +2680,7 @@
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C26">
@@ -2442,7 +2692,7 @@
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2450,7 +2700,7 @@
       <c r="A29" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C29">
@@ -2470,7 +2720,7 @@
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C32">
@@ -2482,7 +2732,7 @@
       <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C33">
@@ -2494,7 +2744,7 @@
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C34">
@@ -2506,7 +2756,7 @@
       <c r="A35" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2514,7 +2764,7 @@
       <c r="A36" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C36">
@@ -2918,7 +3168,7 @@
       </c>
     </row>
     <row r="16" spans="1:32" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="16" t="s">
         <v>64</v>
       </c>
       <c r="L16">
@@ -2926,7 +3176,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="17" t="s">
         <v>68</v>
       </c>
       <c r="L17">
@@ -2934,7 +3184,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="17" t="s">
         <v>69</v>
       </c>
       <c r="L18">
@@ -2942,7 +3192,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
       <c r="L19">
@@ -2950,7 +3200,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
       <c r="L20">
@@ -2958,37 +3208,37 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="17" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="17" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="17" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="17" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="18" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
+      <c r="A27" s="15"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6:D8 H6:H8">
@@ -3017,7 +3267,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AI14" sqref="AI14"/>
     </sheetView>
   </sheetViews>
@@ -3132,40 +3382,40 @@
         <v>4</v>
       </c>
       <c r="F2">
-        <f>B2+D2</f>
+        <f t="shared" ref="F2:G4" si="0">B2+D2</f>
         <v>12</v>
       </c>
       <c r="G2">
-        <f>C2+E2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="M2">
         <v>1</v>
       </c>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21" t="s">
+      <c r="N2" s="19"/>
+      <c r="O2" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24" t="s">
+      <c r="P2" s="21"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="V2" s="24"/>
-      <c r="W2" s="24"/>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="24"/>
-      <c r="AA2" s="24"/>
-      <c r="AB2" s="24"/>
-      <c r="AC2" s="24"/>
-      <c r="AD2" s="24"/>
-      <c r="AE2" s="24"/>
-      <c r="AF2" s="24"/>
-      <c r="AG2" s="24"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22"/>
+      <c r="AA2" s="22"/>
+      <c r="AB2" s="22"/>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="22"/>
+      <c r="AE2" s="22"/>
+      <c r="AF2" s="22"/>
+      <c r="AG2" s="22"/>
       <c r="AI2" t="s">
         <v>102</v>
       </c>
@@ -3187,36 +3437,36 @@
         <v>4</v>
       </c>
       <c r="F3">
-        <f>B3+D3</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="G3">
-        <f>C3+E3</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="M3">
         <v>2</v>
       </c>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="24"/>
-      <c r="Z3" s="24"/>
-      <c r="AA3" s="24"/>
-      <c r="AB3" s="24"/>
-      <c r="AC3" s="24"/>
-      <c r="AD3" s="24"/>
-      <c r="AE3" s="24"/>
-      <c r="AF3" s="24"/>
-      <c r="AG3" s="24"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="22"/>
+      <c r="Y3" s="22"/>
+      <c r="Z3" s="22"/>
+      <c r="AA3" s="22"/>
+      <c r="AB3" s="22"/>
+      <c r="AC3" s="22"/>
+      <c r="AD3" s="22"/>
+      <c r="AE3" s="22"/>
+      <c r="AF3" s="22"/>
+      <c r="AG3" s="22"/>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -3235,65 +3485,65 @@
         <v>6</v>
       </c>
       <c r="F4">
-        <f>B4+D4</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="G4">
-        <f>C4+E4</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="M4">
         <v>3</v>
       </c>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="24"/>
-      <c r="T4" s="24"/>
-      <c r="U4" s="24"/>
-      <c r="V4" s="24"/>
-      <c r="W4" s="24"/>
-      <c r="X4" s="24"/>
-      <c r="Y4" s="24"/>
-      <c r="Z4" s="24"/>
-      <c r="AA4" s="24"/>
-      <c r="AB4" s="24"/>
-      <c r="AC4" s="24"/>
-      <c r="AD4" s="24"/>
-      <c r="AE4" s="24"/>
-      <c r="AF4" s="24"/>
-      <c r="AG4" s="24"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22"/>
+      <c r="AE4" s="22"/>
+      <c r="AF4" s="22"/>
+      <c r="AG4" s="22"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="M5">
         <v>4</v>
       </c>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="24"/>
-      <c r="U5" s="24"/>
-      <c r="V5" s="24"/>
-      <c r="W5" s="24"/>
-      <c r="X5" s="24" t="s">
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="22"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="Y5" s="24" t="s">
+      <c r="Y5" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="Z5" s="24"/>
-      <c r="AA5" s="24"/>
-      <c r="AB5" s="24"/>
-      <c r="AC5" s="24"/>
-      <c r="AD5" s="24"/>
-      <c r="AE5" s="24"/>
-      <c r="AF5" s="24"/>
-      <c r="AG5" s="24"/>
+      <c r="Z5" s="22"/>
+      <c r="AA5" s="22"/>
+      <c r="AB5" s="22"/>
+      <c r="AC5" s="22"/>
+      <c r="AD5" s="22"/>
+      <c r="AE5" s="22"/>
+      <c r="AF5" s="22"/>
+      <c r="AG5" s="22"/>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -3306,26 +3556,26 @@
       <c r="M6">
         <v>5</v>
       </c>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="24"/>
-      <c r="X6" s="24"/>
-      <c r="Y6" s="24"/>
-      <c r="Z6" s="24"/>
-      <c r="AA6" s="24"/>
-      <c r="AB6" s="24"/>
-      <c r="AC6" s="24"/>
-      <c r="AD6" s="24"/>
-      <c r="AE6" s="24"/>
-      <c r="AF6" s="24"/>
-      <c r="AG6" s="23"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="22"/>
+      <c r="Y6" s="22"/>
+      <c r="Z6" s="22"/>
+      <c r="AA6" s="22"/>
+      <c r="AB6" s="22"/>
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="22"/>
+      <c r="AE6" s="22"/>
+      <c r="AF6" s="22"/>
+      <c r="AG6" s="21"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -3338,562 +3588,653 @@
       <c r="M7">
         <v>6</v>
       </c>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="24"/>
-      <c r="W7" s="24"/>
-      <c r="X7" s="24"/>
-      <c r="Y7" s="24"/>
-      <c r="Z7" s="24"/>
-      <c r="AA7" s="24"/>
-      <c r="AB7" s="24"/>
-      <c r="AC7" s="24"/>
-      <c r="AD7" s="24"/>
-      <c r="AE7" s="24"/>
-      <c r="AF7" s="23"/>
-      <c r="AG7" s="25"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="22"/>
+      <c r="W7" s="22"/>
+      <c r="X7" s="22"/>
+      <c r="Y7" s="22"/>
+      <c r="Z7" s="22"/>
+      <c r="AA7" s="22"/>
+      <c r="AB7" s="22"/>
+      <c r="AC7" s="22"/>
+      <c r="AD7" s="22"/>
+      <c r="AE7" s="22"/>
+      <c r="AF7" s="21"/>
+      <c r="AG7" s="23"/>
     </row>
     <row r="8" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M8">
         <v>7</v>
       </c>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="22"/>
-      <c r="T8" s="21"/>
-      <c r="U8" s="21"/>
-      <c r="V8" s="23"/>
-      <c r="W8" s="24"/>
-      <c r="X8" s="24"/>
-      <c r="Y8" s="24"/>
-      <c r="Z8" s="24"/>
-      <c r="AA8" s="24"/>
-      <c r="AB8" s="24"/>
-      <c r="AC8" s="24"/>
-      <c r="AD8" s="24"/>
-      <c r="AE8" s="23"/>
-      <c r="AF8" s="25"/>
-      <c r="AG8" s="25"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="22"/>
+      <c r="X8" s="22"/>
+      <c r="Y8" s="22"/>
+      <c r="Z8" s="22"/>
+      <c r="AA8" s="22"/>
+      <c r="AB8" s="22"/>
+      <c r="AC8" s="22"/>
+      <c r="AD8" s="22"/>
+      <c r="AE8" s="21"/>
+      <c r="AF8" s="23"/>
+      <c r="AG8" s="23"/>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="9" t="b">
+      <c r="B9" s="7" t="b">
         <f>AND(B6 &lt; 0, B7 &gt; 0)</f>
         <v>0</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="8"/>
       <c r="M9">
         <v>8</v>
       </c>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="23"/>
-      <c r="X9" s="24" t="s">
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="21"/>
+      <c r="X9" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="Y9" s="24"/>
-      <c r="Z9" s="24"/>
-      <c r="AA9" s="24"/>
-      <c r="AB9" s="24"/>
-      <c r="AC9" s="24"/>
-      <c r="AD9" s="23"/>
-      <c r="AE9" s="25"/>
-      <c r="AF9" s="25"/>
-      <c r="AG9" s="25"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="21"/>
+      <c r="AE9" s="23"/>
+      <c r="AF9" s="23"/>
+      <c r="AG9" s="23"/>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
       <c r="M10">
         <v>9</v>
       </c>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="21"/>
-      <c r="X10" s="7"/>
-      <c r="Y10" s="7"/>
-      <c r="Z10" s="7"/>
-      <c r="AA10" s="7"/>
-      <c r="AB10" s="7"/>
-      <c r="AC10" s="7"/>
-      <c r="AD10" s="25"/>
-      <c r="AE10" s="25"/>
-      <c r="AF10" s="25"/>
-      <c r="AG10" s="25"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="19"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="23"/>
+      <c r="AE10" s="23"/>
+      <c r="AF10" s="23"/>
+      <c r="AG10" s="23"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="10">
         <f>B4-D2</f>
         <v>6</v>
       </c>
-      <c r="C11" s="13"/>
+      <c r="C11" s="11"/>
       <c r="M11">
         <v>10</v>
       </c>
-      <c r="N11" s="21"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="21"/>
-      <c r="T11" s="21"/>
-      <c r="U11" s="21"/>
-      <c r="V11" s="21"/>
-      <c r="W11" s="21" t="s">
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="X11" s="7"/>
-      <c r="Y11" s="7"/>
-      <c r="Z11" s="7"/>
-      <c r="AA11" s="7" t="s">
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AB11" s="7"/>
-      <c r="AC11" s="7"/>
-      <c r="AD11" s="25"/>
-      <c r="AE11" s="25"/>
-      <c r="AF11" s="25"/>
-      <c r="AG11" s="25"/>
+      <c r="AB11" s="5"/>
+      <c r="AC11" s="5"/>
+      <c r="AD11" s="23"/>
+      <c r="AE11" s="23"/>
+      <c r="AF11" s="23"/>
+      <c r="AG11" s="23"/>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
       <c r="M12">
         <v>11</v>
       </c>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21"/>
-      <c r="T12" s="21"/>
-      <c r="U12" s="21"/>
-      <c r="V12" s="21" t="s">
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="W12" s="21"/>
-      <c r="X12" s="7"/>
-      <c r="Y12" s="7"/>
-      <c r="Z12" s="7"/>
-      <c r="AA12" s="7"/>
-      <c r="AB12" s="7"/>
-      <c r="AC12" s="7"/>
-      <c r="AD12" s="25"/>
-      <c r="AE12" s="25"/>
-      <c r="AF12" s="25"/>
-      <c r="AG12" s="25"/>
+      <c r="W12" s="19"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
+      <c r="AB12" s="5"/>
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="23"/>
+      <c r="AE12" s="23"/>
+      <c r="AF12" s="23"/>
+      <c r="AG12" s="23"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="10">
         <f>C2-C3</f>
         <v>-10</v>
       </c>
-      <c r="C13" s="13"/>
+      <c r="C13" s="11"/>
       <c r="M13">
         <v>12</v>
       </c>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="21"/>
-      <c r="S13" s="21"/>
-      <c r="T13" s="21"/>
-      <c r="U13" s="21"/>
-      <c r="V13" s="21"/>
-      <c r="W13" s="21"/>
-      <c r="X13" s="7"/>
-      <c r="Y13" s="7"/>
-      <c r="Z13" s="7"/>
-      <c r="AA13" s="7"/>
-      <c r="AB13" s="7"/>
-      <c r="AC13" s="7"/>
-      <c r="AD13" s="25"/>
-      <c r="AE13" s="25"/>
-      <c r="AF13" s="25"/>
-      <c r="AG13" s="25"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="19"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="5"/>
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="23"/>
+      <c r="AE13" s="23"/>
+      <c r="AF13" s="23"/>
+      <c r="AG13" s="23"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="10">
         <f>B2-B3</f>
         <v>-5</v>
       </c>
-      <c r="C14" s="13"/>
+      <c r="C14" s="11"/>
       <c r="M14">
         <v>13</v>
       </c>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21"/>
-      <c r="S14" s="21"/>
-      <c r="T14" s="21"/>
-      <c r="U14" s="21"/>
-      <c r="V14" s="21"/>
-      <c r="W14" s="21"/>
-      <c r="X14" s="7"/>
-      <c r="Y14" s="7"/>
-      <c r="Z14" s="7"/>
-      <c r="AA14" s="7"/>
-      <c r="AB14" s="7"/>
-      <c r="AC14" s="7"/>
-      <c r="AD14" s="25"/>
-      <c r="AE14" s="25"/>
-      <c r="AF14" s="25"/>
-      <c r="AG14" s="25"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="23"/>
+      <c r="AE14" s="23"/>
+      <c r="AF14" s="23"/>
+      <c r="AG14" s="23"/>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
       <c r="M15">
         <v>14</v>
       </c>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="21"/>
-      <c r="S15" s="22"/>
-      <c r="T15" s="21"/>
-      <c r="U15" s="21"/>
-      <c r="V15" s="21"/>
-      <c r="W15" s="21"/>
-      <c r="X15" s="7"/>
-      <c r="Y15" s="7"/>
-      <c r="Z15" s="7"/>
-      <c r="AA15" s="7"/>
-      <c r="AB15" s="7"/>
-      <c r="AC15" s="7"/>
-      <c r="AD15" s="25"/>
-      <c r="AE15" s="25"/>
-      <c r="AF15" s="25"/>
-      <c r="AG15" s="25"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="19"/>
+      <c r="W15" s="19"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="5"/>
+      <c r="AC15" s="5"/>
+      <c r="AD15" s="23"/>
+      <c r="AE15" s="23"/>
+      <c r="AF15" s="23"/>
+      <c r="AG15" s="23"/>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="10">
         <f>ATAN(B13/B14)</f>
         <v>1.1071487177940904</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="11">
         <f>DEGREES(B16)</f>
         <v>63.43494882292201</v>
       </c>
       <c r="M16">
         <v>15</v>
       </c>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="21"/>
-      <c r="S16" s="21"/>
-      <c r="T16" s="21"/>
-      <c r="U16" s="21"/>
-      <c r="V16" s="21"/>
-      <c r="W16" s="23"/>
-      <c r="X16" s="26"/>
-      <c r="Y16" s="26"/>
-      <c r="Z16" s="26"/>
-      <c r="AA16" s="26"/>
-      <c r="AB16" s="26"/>
-      <c r="AC16" s="26"/>
-      <c r="AD16" s="23"/>
-      <c r="AE16" s="25"/>
-      <c r="AF16" s="25"/>
-      <c r="AG16" s="25"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+      <c r="V16" s="19"/>
+      <c r="W16" s="21"/>
+      <c r="X16" s="24"/>
+      <c r="Y16" s="24"/>
+      <c r="Z16" s="24"/>
+      <c r="AA16" s="24"/>
+      <c r="AB16" s="24"/>
+      <c r="AC16" s="24"/>
+      <c r="AD16" s="21"/>
+      <c r="AE16" s="23"/>
+      <c r="AF16" s="23"/>
+      <c r="AG16" s="23"/>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
       <c r="M17">
         <v>16</v>
       </c>
-      <c r="N17" s="21"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="21"/>
-      <c r="S17" s="21"/>
-      <c r="T17" s="21"/>
-      <c r="U17" s="21"/>
-      <c r="V17" s="23"/>
-      <c r="W17" s="26"/>
-      <c r="X17" s="26"/>
-      <c r="Y17" s="26"/>
-      <c r="Z17" s="26"/>
-      <c r="AA17" s="26"/>
-      <c r="AB17" s="26"/>
-      <c r="AC17" s="26"/>
-      <c r="AD17" s="26"/>
-      <c r="AE17" s="23"/>
-      <c r="AF17" s="25"/>
-      <c r="AG17" s="25"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="21"/>
+      <c r="W17" s="24"/>
+      <c r="X17" s="24"/>
+      <c r="Y17" s="24"/>
+      <c r="Z17" s="24"/>
+      <c r="AA17" s="24"/>
+      <c r="AB17" s="24"/>
+      <c r="AC17" s="24"/>
+      <c r="AD17" s="24"/>
+      <c r="AE17" s="21"/>
+      <c r="AF17" s="23"/>
+      <c r="AG17" s="23"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="10">
         <f>B3-B11</f>
         <v>7</v>
       </c>
-      <c r="C18" s="13"/>
+      <c r="C18" s="11"/>
       <c r="M18">
         <v>17</v>
       </c>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="21"/>
-      <c r="S18" s="21"/>
-      <c r="T18" s="21"/>
-      <c r="U18" s="23"/>
-      <c r="V18" s="26"/>
-      <c r="W18" s="26"/>
-      <c r="X18" s="26"/>
-      <c r="Y18" s="26"/>
-      <c r="Z18" s="26"/>
-      <c r="AA18" s="26"/>
-      <c r="AB18" s="26"/>
-      <c r="AC18" s="26"/>
-      <c r="AD18" s="26"/>
-      <c r="AE18" s="26"/>
-      <c r="AF18" s="23"/>
-      <c r="AG18" s="25"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="21"/>
+      <c r="V18" s="24"/>
+      <c r="W18" s="24"/>
+      <c r="X18" s="24"/>
+      <c r="Y18" s="24"/>
+      <c r="Z18" s="24"/>
+      <c r="AA18" s="24"/>
+      <c r="AB18" s="24"/>
+      <c r="AC18" s="24"/>
+      <c r="AD18" s="24"/>
+      <c r="AE18" s="24"/>
+      <c r="AF18" s="21"/>
+      <c r="AG18" s="23"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
       <c r="M19">
         <v>18</v>
       </c>
-      <c r="N19" s="21"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
-      <c r="T19" s="23"/>
-      <c r="U19" s="26"/>
-      <c r="V19" s="26"/>
-      <c r="W19" s="26"/>
-      <c r="X19" s="26"/>
-      <c r="Y19" s="26"/>
-      <c r="Z19" s="26"/>
-      <c r="AA19" s="26"/>
-      <c r="AB19" s="26"/>
-      <c r="AC19" s="26"/>
-      <c r="AD19" s="26"/>
-      <c r="AE19" s="26"/>
-      <c r="AF19" s="26"/>
-      <c r="AG19" s="23"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="21"/>
+      <c r="U19" s="24"/>
+      <c r="V19" s="24"/>
+      <c r="W19" s="24"/>
+      <c r="X19" s="24"/>
+      <c r="Y19" s="24"/>
+      <c r="Z19" s="24"/>
+      <c r="AA19" s="24"/>
+      <c r="AB19" s="24"/>
+      <c r="AC19" s="24"/>
+      <c r="AD19" s="24"/>
+      <c r="AE19" s="24"/>
+      <c r="AF19" s="24"/>
+      <c r="AG19" s="21"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
       <c r="M20">
         <v>19</v>
       </c>
-      <c r="N20" s="21"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="21"/>
-      <c r="S20" s="23"/>
-      <c r="T20" s="26"/>
-      <c r="U20" s="26"/>
-      <c r="V20" s="26"/>
-      <c r="W20" s="26"/>
-      <c r="X20" s="26"/>
-      <c r="Y20" s="26"/>
-      <c r="Z20" s="26"/>
-      <c r="AA20" s="26"/>
-      <c r="AB20" s="26"/>
-      <c r="AC20" s="26"/>
-      <c r="AD20" s="26"/>
-      <c r="AE20" s="26"/>
-      <c r="AF20" s="26"/>
-      <c r="AG20" s="26"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="24"/>
+      <c r="U20" s="24"/>
+      <c r="V20" s="24"/>
+      <c r="W20" s="24"/>
+      <c r="X20" s="24"/>
+      <c r="Y20" s="24"/>
+      <c r="Z20" s="24"/>
+      <c r="AA20" s="24"/>
+      <c r="AB20" s="24"/>
+      <c r="AC20" s="24"/>
+      <c r="AD20" s="24"/>
+      <c r="AE20" s="24"/>
+      <c r="AF20" s="24"/>
+      <c r="AG20" s="24"/>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="10">
         <f>B18*TAN(B16)</f>
         <v>13.999999999999996</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="N21" s="21"/>
-      <c r="O21" s="21"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="23"/>
-      <c r="S21" s="26"/>
-      <c r="T21" s="26"/>
-      <c r="U21" s="26"/>
-      <c r="V21" s="26"/>
-      <c r="W21" s="26"/>
-      <c r="X21" s="26"/>
-      <c r="Y21" s="26"/>
-      <c r="Z21" s="26"/>
-      <c r="AA21" s="26"/>
-      <c r="AB21" s="26"/>
-      <c r="AC21" s="26"/>
-      <c r="AD21" s="26"/>
-      <c r="AE21" s="26"/>
-      <c r="AF21" s="26"/>
-      <c r="AG21" s="26"/>
+      <c r="C21" s="11"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="24"/>
+      <c r="W21" s="24"/>
+      <c r="X21" s="24"/>
+      <c r="Y21" s="24"/>
+      <c r="Z21" s="24"/>
+      <c r="AA21" s="24"/>
+      <c r="AB21" s="24"/>
+      <c r="AC21" s="24"/>
+      <c r="AD21" s="24"/>
+      <c r="AE21" s="24"/>
+      <c r="AF21" s="24"/>
+      <c r="AG21" s="24"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="23"/>
-      <c r="R22" s="26"/>
-      <c r="S22" s="26"/>
-      <c r="T22" s="26"/>
-      <c r="U22" s="26"/>
-      <c r="V22" s="26"/>
-      <c r="W22" s="26"/>
-      <c r="X22" s="26"/>
-      <c r="Y22" s="26"/>
-      <c r="Z22" s="26"/>
-      <c r="AA22" s="26"/>
-      <c r="AB22" s="26"/>
-      <c r="AC22" s="26"/>
-      <c r="AD22" s="26"/>
-      <c r="AE22" s="26"/>
-      <c r="AF22" s="26"/>
-      <c r="AG22" s="26"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="21"/>
+      <c r="R22" s="24"/>
+      <c r="S22" s="24"/>
+      <c r="T22" s="24"/>
+      <c r="U22" s="24"/>
+      <c r="V22" s="24"/>
+      <c r="W22" s="24"/>
+      <c r="X22" s="24"/>
+      <c r="Y22" s="24"/>
+      <c r="Z22" s="24"/>
+      <c r="AA22" s="24"/>
+      <c r="AB22" s="24"/>
+      <c r="AC22" s="24"/>
+      <c r="AD22" s="24"/>
+      <c r="AE22" s="24"/>
+      <c r="AF22" s="24"/>
+      <c r="AG22" s="24"/>
     </row>
     <row r="23" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B23" s="15">
+      <c r="B23" s="13">
         <f>C3-B21</f>
         <v>-3.9999999999999964</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="N23" s="21"/>
-      <c r="O23" s="21"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="26"/>
-      <c r="R23" s="26"/>
-      <c r="S23" s="26"/>
-      <c r="T23" s="26"/>
-      <c r="U23" s="26"/>
-      <c r="V23" s="26"/>
-      <c r="W23" s="26"/>
-      <c r="X23" s="26"/>
-      <c r="Y23" s="26"/>
-      <c r="Z23" s="26"/>
-      <c r="AA23" s="26"/>
-      <c r="AB23" s="26"/>
-      <c r="AC23" s="26"/>
-      <c r="AD23" s="26"/>
-      <c r="AE23" s="26"/>
-      <c r="AF23" s="26"/>
-      <c r="AG23" s="26"/>
+      <c r="C23" s="14"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="21"/>
+      <c r="Q23" s="24"/>
+      <c r="R23" s="24"/>
+      <c r="S23" s="24"/>
+      <c r="T23" s="24"/>
+      <c r="U23" s="24"/>
+      <c r="V23" s="24"/>
+      <c r="W23" s="24"/>
+      <c r="X23" s="24"/>
+      <c r="Y23" s="24"/>
+      <c r="Z23" s="24"/>
+      <c r="AA23" s="24"/>
+      <c r="AB23" s="24"/>
+      <c r="AC23" s="24"/>
+      <c r="AD23" s="24"/>
+      <c r="AE23" s="24"/>
+      <c r="AF23" s="24"/>
+      <c r="AG23" s="24"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="N24" s="21"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="26"/>
-      <c r="S24" s="26"/>
-      <c r="T24" s="26"/>
-      <c r="U24" s="26"/>
-      <c r="V24" s="26"/>
-      <c r="W24" s="26"/>
-      <c r="X24" s="26"/>
-      <c r="Y24" s="26"/>
-      <c r="Z24" s="26"/>
-      <c r="AA24" s="26"/>
-      <c r="AB24" s="26"/>
-      <c r="AC24" s="26"/>
-      <c r="AD24" s="26"/>
-      <c r="AE24" s="26"/>
-      <c r="AF24" s="26"/>
-      <c r="AG24" s="26"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="24"/>
+      <c r="Q24" s="24"/>
+      <c r="R24" s="24"/>
+      <c r="S24" s="24"/>
+      <c r="T24" s="24"/>
+      <c r="U24" s="24"/>
+      <c r="V24" s="24"/>
+      <c r="W24" s="24"/>
+      <c r="X24" s="24"/>
+      <c r="Y24" s="24"/>
+      <c r="Z24" s="24"/>
+      <c r="AA24" s="24"/>
+      <c r="AB24" s="24"/>
+      <c r="AC24" s="24"/>
+      <c r="AD24" s="24"/>
+      <c r="AE24" s="24"/>
+      <c r="AF24" s="24"/>
+      <c r="AG24" s="24"/>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="N25" s="23"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="26"/>
-      <c r="R25" s="26"/>
-      <c r="S25" s="26"/>
-      <c r="T25" s="26"/>
-      <c r="U25" s="26"/>
-      <c r="V25" s="26"/>
-      <c r="W25" s="26"/>
-      <c r="X25" s="26"/>
-      <c r="Y25" s="26"/>
-      <c r="Z25" s="26"/>
-      <c r="AA25" s="26"/>
-      <c r="AB25" s="26"/>
-      <c r="AC25" s="26"/>
-      <c r="AD25" s="26"/>
-      <c r="AE25" s="26"/>
-      <c r="AF25" s="26"/>
-      <c r="AG25" s="26"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="24"/>
+      <c r="S25" s="24"/>
+      <c r="T25" s="24"/>
+      <c r="U25" s="24"/>
+      <c r="V25" s="24"/>
+      <c r="W25" s="24"/>
+      <c r="X25" s="24"/>
+      <c r="Y25" s="24"/>
+      <c r="Z25" s="24"/>
+      <c r="AA25" s="24"/>
+      <c r="AB25" s="24"/>
+      <c r="AC25" s="24"/>
+      <c r="AD25" s="24"/>
+      <c r="AE25" s="24"/>
+      <c r="AF25" s="24"/>
+      <c r="AG25" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <f>B6/B2</f>
+        <v>0.11428571428571428</v>
+      </c>
+      <c r="C8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <f>B7/B3</f>
+        <v>0.6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Monsters are able to "see" Zero if he is around
Logic for detecting Zero by each monster added. Movement hasn't implemented yet though.
Bug fix from the previous update when there were not transfering data correctly of reading the monsters_info.dat file
</commit_message>
<xml_diff>
--- a/calcs.xlsx
+++ b/calcs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8136"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8136" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="frames" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="colide" sheetId="6" r:id="rId5"/>
     <sheet name="process wall colision" sheetId="7" r:id="rId6"/>
     <sheet name="scaleSpriteTo" sheetId="8" r:id="rId7"/>
+    <sheet name="monsters" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="137">
   <si>
     <t>y \ x</t>
   </si>
@@ -514,6 +515,66 @@
   </si>
   <si>
     <t>column</t>
+  </si>
+  <si>
+    <t>How monsters look for Zero</t>
+  </si>
+  <si>
+    <t>window width</t>
+  </si>
+  <si>
+    <t>window heigth</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>monster.x</t>
+  </si>
+  <si>
+    <t>monster.y</t>
+  </si>
+  <si>
+    <t>monster.w</t>
+  </si>
+  <si>
+    <t>single block width</t>
+  </si>
+  <si>
+    <t>single block heigth</t>
+  </si>
+  <si>
+    <t>monster.h</t>
+  </si>
+  <si>
+    <t>angle</t>
+  </si>
+  <si>
+    <t>multiplier</t>
+  </si>
+  <si>
+    <t>place.w</t>
+  </si>
+  <si>
+    <t>place.h</t>
+  </si>
+  <si>
+    <t>monster.center.x</t>
+  </si>
+  <si>
+    <t>monster.center.y</t>
+  </si>
+  <si>
+    <t>place.x</t>
+  </si>
+  <si>
+    <t>place.y</t>
+  </si>
+  <si>
+    <t>angle precision</t>
+  </si>
+  <si>
+    <t>multiplier precision</t>
   </si>
 </sst>
 </file>
@@ -564,7 +625,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -616,6 +677,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -727,7 +794,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -779,6 +846,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -926,11 +1001,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="293212544"/>
-        <c:axId val="293214080"/>
+        <c:axId val="297273984"/>
+        <c:axId val="281600384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="293212544"/>
+        <c:axId val="297273984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="800"/>
@@ -941,13 +1016,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="293214080"/>
+        <c:crossAx val="281600384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="293214080"/>
+        <c:axId val="281600384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -958,9 +1033,368 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="293212544"/>
+        <c:crossAx val="297273984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>monsters!$D$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>place.y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="50"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>monsters!$C$12:$C$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>685.71428571428578</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>664.7284391812068</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>606.90896672025258</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>526.41209171446337</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>442.94625659191848</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>376.94680876338282</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>344.5727148684951</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>353.75028217872068</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>402.23252213766659</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>478.14929152615207</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>562.91351750798174</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>635.77196130707318</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>678.88633485434855</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>771.42857142857156</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>739.94980162895308</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>653.2205929375217</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>532.47528042883789</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>407.27652774502053</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>308.27735600221706</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>259.71621515988545</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>273.4825661252238</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>346.20592606364266</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>460.08108014637099</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>587.22741911911544</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>696.51508481775261</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>761.18664513866565</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>857.14285714285722</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>815.17116407669937</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>699.53221915479082</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>538.53846914321252</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>371.60679889812263</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>239.6079032410513</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>174.85971545127586</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>193.21485007172697</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>290.17932998961879</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>442.01286876658986</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>611.54132073024903</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>757.25820832843203</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>843.48695542298265</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>monsters!$D$12:$D$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>385.71428571428567</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>447.35471210625462</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>493.90341233244379</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>513.96364113480695</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>502.62395487758761</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>462.6607042419372</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>403.85828675055433</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>340.61358501133452</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>288.41110774612349</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>260.03184201448749</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>262.42402182902504</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>295.00195814094957</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>349.78943594585235</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>385.71428571428567</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>478.1749253022391</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>547.99797564152277</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>578.08831884506753</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>561.07878945923858</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>501.13391350576296</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>412.93028726868863</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>318.06323465985901</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>239.75951876204238</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>197.19062016458841</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>200.77888988639469</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>249.64579435428152</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>331.82701106163569</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>385.71428571428567</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>508.99513849822358</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>602.09253895060192</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>642.21299655532823</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>619.53362404088944</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>539.60712276958873</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>422.00228778682293</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>295.51288430838343</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>191.10792977796129</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>134.34939831468932</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>139.13375794376438</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>204.28963056761347</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>313.86458617741903</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="141656064"/>
+        <c:axId val="141654272"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="141656064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="141654272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="114"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="141654272"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="141656064"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="85"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -1691,6 +2125,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>354330</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>415290</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема на Office">
   <a:themeElements>
@@ -1946,7 +2415,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1956,7 +2425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -4237,4 +4706,994 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="11" max="11" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="34.44140625" customWidth="1"/>
+    <col min="20" max="20" width="26.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1">
+        <v>800</v>
+      </c>
+      <c r="N1" t="s">
+        <v>124</v>
+      </c>
+      <c r="O1">
+        <f>L1/7</f>
+        <v>114.28571428571429</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="31">
+        <f>O1</f>
+        <v>114.28571428571429</v>
+      </c>
+      <c r="C2" s="31">
+        <f>B2+$O1</f>
+        <v>228.57142857142858</v>
+      </c>
+      <c r="D2" s="31">
+        <f>C2+$O1</f>
+        <v>342.85714285714289</v>
+      </c>
+      <c r="E2" s="31">
+        <f>D2+$O1</f>
+        <v>457.14285714285717</v>
+      </c>
+      <c r="F2" s="31">
+        <f>E2+$O1</f>
+        <v>571.42857142857144</v>
+      </c>
+      <c r="G2" s="31">
+        <f>F2+$O1</f>
+        <v>685.71428571428578</v>
+      </c>
+      <c r="H2" s="31">
+        <f>G2+$O1</f>
+        <v>800.00000000000011</v>
+      </c>
+      <c r="K2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L2">
+        <v>600</v>
+      </c>
+      <c r="N2" t="s">
+        <v>125</v>
+      </c>
+      <c r="O2">
+        <f>L2/7</f>
+        <v>85.714285714285708</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="31">
+        <f>O2</f>
+        <v>85.714285714285708</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="K3" t="s">
+        <v>121</v>
+      </c>
+      <c r="L3" s="31">
+        <f>E2</f>
+        <v>457.14285714285717</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="31">
+        <f>A3+O$2</f>
+        <v>171.42857142857142</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="K4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" s="31">
+        <f>A6</f>
+        <v>342.85714285714283</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="31">
+        <f>A4+O$2</f>
+        <v>257.14285714285711</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="K5" t="s">
+        <v>123</v>
+      </c>
+      <c r="L5">
+        <f>O1</f>
+        <v>114.28571428571429</v>
+      </c>
+      <c r="N5" t="s">
+        <v>131</v>
+      </c>
+      <c r="O5">
+        <f>L3+(L5/2)</f>
+        <v>514.28571428571433</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="31">
+        <f>A5+O$2</f>
+        <v>342.85714285714283</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="K6" t="s">
+        <v>126</v>
+      </c>
+      <c r="L6">
+        <f>O2</f>
+        <v>85.714285714285708</v>
+      </c>
+      <c r="N6" t="s">
+        <v>132</v>
+      </c>
+      <c r="O6">
+        <f>L4+(L6/2)</f>
+        <v>385.71428571428567</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="31">
+        <f>A6+O$2</f>
+        <v>428.57142857142856</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="K7" t="s">
+        <v>127</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="31">
+        <f>A7+O$2</f>
+        <v>514.28571428571422</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="K8" t="s">
+        <v>128</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="31">
+        <f>A8+O$2</f>
+        <v>599.99999999999989</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="5"/>
+      <c r="K9" t="s">
+        <v>129</v>
+      </c>
+      <c r="L9">
+        <f>L5</f>
+        <v>114.28571428571429</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K10" t="s">
+        <v>130</v>
+      </c>
+      <c r="L10">
+        <f>L6</f>
+        <v>85.714285714285708</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F11" t="s">
+        <v>135</v>
+      </c>
+      <c r="H11" t="s">
+        <v>136</v>
+      </c>
+      <c r="K11" t="s">
+        <v>133</v>
+      </c>
+      <c r="L11">
+        <f>O5 + 1.5*L5*COS(L7)*L8</f>
+        <v>685.71428571428578</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <f>O$5 + 1.5*L$5*COS(A12)*B12</f>
+        <v>685.71428571428578</v>
+      </c>
+      <c r="D12">
+        <f>O$6+1.5*L$6*SIN(A12)*B12</f>
+        <v>385.71428571428567</v>
+      </c>
+      <c r="F12">
+        <v>0.5</v>
+      </c>
+      <c r="H12">
+        <v>0.5</v>
+      </c>
+      <c r="K12" t="s">
+        <v>134</v>
+      </c>
+      <c r="L12">
+        <f>O6+1.5*L6*SIN(L7)*L8</f>
+        <v>385.71428571428567</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f>IF(A12=6,0,A12+F$12)</f>
+        <v>0.5</v>
+      </c>
+      <c r="B13">
+        <f>IF(A12=6,B12+H$12,B12)</f>
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <f>O$5 + 1.5*L$5*COS(A13)*B13</f>
+        <v>664.7284391812068</v>
+      </c>
+      <c r="D13">
+        <f>O$6+1.5*L$6*SIN(A13)*B13</f>
+        <v>447.35471210625462</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" ref="A14:A25" si="0">IF(A13=6,0,A13+F$12)</f>
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:B21" si="1">IF(A13=6,B13+H$12,B13)</f>
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:C21" si="2">O$5 + 1.5*L$5*COS(A14)*B14</f>
+        <v>606.90896672025258</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:D21" si="3">O$6+1.5*L$6*SIN(A14)*B14</f>
+        <v>493.90341233244379</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="2"/>
+        <v>526.41209171446337</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="3"/>
+        <v>513.96364113480695</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="2"/>
+        <v>442.94625659191848</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="3"/>
+        <v>502.62395487758761</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="2"/>
+        <v>376.94680876338282</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="3"/>
+        <v>462.6607042419372</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="2"/>
+        <v>344.5727148684951</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="3"/>
+        <v>403.85828675055433</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="2"/>
+        <v>353.75028217872068</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="3"/>
+        <v>340.61358501133452</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="2"/>
+        <v>402.23252213766659</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="3"/>
+        <v>288.41110774612349</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="2"/>
+        <v>478.14929152615207</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="3"/>
+        <v>260.03184201448749</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <f>IF(A21=6,B21+H$12,B21)</f>
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <f>O$5 + 1.5*L$5*COS(A22)*B22</f>
+        <v>562.91351750798174</v>
+      </c>
+      <c r="D22">
+        <f>O$6+1.5*L$6*SIN(A22)*B22</f>
+        <v>262.42402182902504</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+      <c r="B23">
+        <f t="shared" ref="B23:B24" si="4">IF(A22=6,B22+H$12,B22)</f>
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:C24" si="5">O$5 + 1.5*L$5*COS(A23)*B23</f>
+        <v>635.77196130707318</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ref="D23:D24" si="6">O$6+1.5*L$6*SIN(A23)*B23</f>
+        <v>295.00195814094957</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="5"/>
+        <v>678.88633485434855</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="6"/>
+        <v>349.78943594585235</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <f>IF(A24=6,B24+H$12,B24)</f>
+        <v>1.5</v>
+      </c>
+      <c r="C25">
+        <f>O$5 + 1.5*L$5*COS(A25)*B25</f>
+        <v>771.42857142857156</v>
+      </c>
+      <c r="D25">
+        <f>O$6+1.5*L$6*SIN(A25)*B25</f>
+        <v>385.71428571428567</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" ref="A26:A37" si="7">IF(A25=6,0,A25+F$12)</f>
+        <v>0.5</v>
+      </c>
+      <c r="B26">
+        <f t="shared" ref="B26:B36" si="8">IF(A25=6,B25+H$12,B25)</f>
+        <v>1.5</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ref="C26:C36" si="9">O$5 + 1.5*L$5*COS(A26)*B26</f>
+        <v>739.94980162895308</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ref="D26:D36" si="10">O$6+1.5*L$6*SIN(A26)*B26</f>
+        <v>478.1749253022391</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="8"/>
+        <v>1.5</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="9"/>
+        <v>653.2205929375217</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="10"/>
+        <v>547.99797564152277</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f t="shared" si="7"/>
+        <v>1.5</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="8"/>
+        <v>1.5</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="9"/>
+        <v>532.47528042883789</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="10"/>
+        <v>578.08831884506753</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="8"/>
+        <v>1.5</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="9"/>
+        <v>407.27652774502053</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="10"/>
+        <v>561.07878945923858</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="8"/>
+        <v>1.5</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="9"/>
+        <v>308.27735600221706</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="10"/>
+        <v>501.13391350576296</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="8"/>
+        <v>1.5</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="9"/>
+        <v>259.71621515988545</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="10"/>
+        <v>412.93028726868863</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" si="7"/>
+        <v>3.5</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="8"/>
+        <v>1.5</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="9"/>
+        <v>273.4825661252238</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="10"/>
+        <v>318.06323465985901</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="8"/>
+        <v>1.5</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="9"/>
+        <v>346.20592606364266</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="10"/>
+        <v>239.75951876204238</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" si="7"/>
+        <v>4.5</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="8"/>
+        <v>1.5</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="9"/>
+        <v>460.08108014637099</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="10"/>
+        <v>197.19062016458841</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="8"/>
+        <v>1.5</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="9"/>
+        <v>587.22741911911544</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="10"/>
+        <v>200.77888988639469</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" si="7"/>
+        <v>5.5</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="8"/>
+        <v>1.5</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="9"/>
+        <v>696.51508481775261</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="10"/>
+        <v>249.64579435428152</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="B37">
+        <f>IF(A36=6,B36+H$12,B36)</f>
+        <v>1.5</v>
+      </c>
+      <c r="C37">
+        <f>O$5 + 1.5*L$5*COS(A37)*B37</f>
+        <v>761.18664513866565</v>
+      </c>
+      <c r="D37">
+        <f>O$6+1.5*L$6*SIN(A37)*B37</f>
+        <v>331.82701106163569</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <f t="shared" ref="A38:A52" si="11">IF(A37=6,0,A37+F$12)</f>
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <f t="shared" ref="B38:B52" si="12">IF(A37=6,B37+H$12,B37)</f>
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <f t="shared" ref="C38:C52" si="13">O$5 + 1.5*L$5*COS(A38)*B38</f>
+        <v>857.14285714285722</v>
+      </c>
+      <c r="D38">
+        <f t="shared" ref="D38:D52" si="14">O$6+1.5*L$6*SIN(A38)*B38</f>
+        <v>385.71428571428567</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <f t="shared" si="11"/>
+        <v>0.5</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="13"/>
+        <v>815.17116407669937</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="14"/>
+        <v>508.99513849822358</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="13"/>
+        <v>699.53221915479082</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="14"/>
+        <v>602.09253895060192</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <f t="shared" si="11"/>
+        <v>1.5</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="13"/>
+        <v>538.53846914321252</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="14"/>
+        <v>642.21299655532823</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="13"/>
+        <v>371.60679889812263</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="14"/>
+        <v>619.53362404088944</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <f t="shared" si="11"/>
+        <v>2.5</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="13"/>
+        <v>239.6079032410513</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="14"/>
+        <v>539.60712276958873</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="13"/>
+        <v>174.85971545127586</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="14"/>
+        <v>422.00228778682293</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <f t="shared" si="11"/>
+        <v>3.5</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="13"/>
+        <v>193.21485007172697</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="14"/>
+        <v>295.51288430838343</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="13"/>
+        <v>290.17932998961879</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="14"/>
+        <v>191.10792977796129</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <f t="shared" si="11"/>
+        <v>4.5</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="13"/>
+        <v>442.01286876658986</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="14"/>
+        <v>134.34939831468932</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="13"/>
+        <v>611.54132073024903</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="14"/>
+        <v>139.13375794376438</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <f t="shared" si="11"/>
+        <v>5.5</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="13"/>
+        <v>757.25820832843203</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="14"/>
+        <v>204.28963056761347</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="13"/>
+        <v>843.48695542298265</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="14"/>
+        <v>313.86458617741903</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Monsters move towards Zero when see him in a close range.
Monsters speed and damage is taken by the monsters_info.dat file but not form code.
Minor refactoring - unnecessary commented out code was removed.
A small improvement how moving objects to behave when colliding a wall
</commit_message>
<xml_diff>
--- a/calcs.xlsx
+++ b/calcs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8136" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8136" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="frames" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="process wall colision" sheetId="7" r:id="rId6"/>
     <sheet name="scaleSpriteTo" sheetId="8" r:id="rId7"/>
     <sheet name="monsters" sheetId="9" r:id="rId8"/>
+    <sheet name="process collisions 2" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="139">
   <si>
     <t>y \ x</t>
   </si>
@@ -575,6 +576,12 @@
   </si>
   <si>
     <t>multiplier precision</t>
+  </si>
+  <si>
+    <t>monster before</t>
+  </si>
+  <si>
+    <t>monster now</t>
   </si>
 </sst>
 </file>
@@ -1001,11 +1008,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="297273984"/>
-        <c:axId val="281600384"/>
+        <c:axId val="275059456"/>
+        <c:axId val="275060992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="297273984"/>
+        <c:axId val="275059456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="800"/>
@@ -1016,13 +1023,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="281600384"/>
+        <c:crossAx val="275060992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="281600384"/>
+        <c:axId val="275060992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1033,7 +1040,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297273984"/>
+        <c:crossAx val="275059456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1359,11 +1366,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="141656064"/>
-        <c:axId val="141654272"/>
+        <c:axId val="275746816"/>
+        <c:axId val="275748352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="141656064"/>
+        <c:axId val="275746816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1374,13 +1381,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141654272"/>
+        <c:crossAx val="275748352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="114"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141654272"/>
+        <c:axId val="275748352"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1391,12 +1398,284 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141656064"/>
+        <c:crossAx val="275746816"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="85"/>
       </c:valAx>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'process collisions 2'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>wall</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'process collisions 2'!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>114</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'process collisions 2'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>425</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>425</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>425</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'process collisions 2'!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>monster before</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'process collisions 2'!$A$8:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'process collisions 2'!$B$8:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>552</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>552</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>510</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'process collisions 2'!$D$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>monster now</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'process collisions 2'!$A$14:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>61</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'process collisions 2'!$B$14:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>552</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>552</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>510</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="43809024"/>
+        <c:axId val="43807488"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="43809024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="43807488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="43807488"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="43809024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2160,6 +2439,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема на Office">
   <a:themeElements>
@@ -2415,7 +2729,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4712,7 +5026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -4751,27 +5065,27 @@
         <v>114.28571428571429</v>
       </c>
       <c r="C2" s="31">
-        <f>B2+$O1</f>
+        <f t="shared" ref="C2:H2" si="0">B2+$O1</f>
         <v>228.57142857142858</v>
       </c>
       <c r="D2" s="31">
-        <f>C2+$O1</f>
+        <f t="shared" si="0"/>
         <v>342.85714285714289</v>
       </c>
       <c r="E2" s="31">
-        <f>D2+$O1</f>
+        <f t="shared" si="0"/>
         <v>457.14285714285717</v>
       </c>
       <c r="F2" s="31">
-        <f>E2+$O1</f>
+        <f t="shared" si="0"/>
         <v>571.42857142857144</v>
       </c>
       <c r="G2" s="31">
-        <f>F2+$O1</f>
+        <f t="shared" si="0"/>
         <v>685.71428571428578</v>
       </c>
       <c r="H2" s="31">
-        <f>G2+$O1</f>
+        <f t="shared" si="0"/>
         <v>800.00000000000011</v>
       </c>
       <c r="K2" t="s">
@@ -4810,7 +5124,7 @@
     </row>
     <row r="4" spans="1:15" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="31">
-        <f>A3+O$2</f>
+        <f t="shared" ref="A4:A9" si="1">A3+O$2</f>
         <v>171.42857142857142</v>
       </c>
       <c r="B4" s="5"/>
@@ -4830,7 +5144,7 @@
     </row>
     <row r="5" spans="1:15" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="31">
-        <f>A4+O$2</f>
+        <f t="shared" si="1"/>
         <v>257.14285714285711</v>
       </c>
       <c r="B5" s="5"/>
@@ -4857,7 +5171,7 @@
     </row>
     <row r="6" spans="1:15" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="31">
-        <f>A5+O$2</f>
+        <f t="shared" si="1"/>
         <v>342.85714285714283</v>
       </c>
       <c r="B6" s="5"/>
@@ -4884,7 +5198,7 @@
     </row>
     <row r="7" spans="1:15" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31">
-        <f>A6+O$2</f>
+        <f t="shared" si="1"/>
         <v>428.57142857142856</v>
       </c>
       <c r="B7" s="5"/>
@@ -4905,7 +5219,7 @@
     </row>
     <row r="8" spans="1:15" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="31">
-        <f>A7+O$2</f>
+        <f t="shared" si="1"/>
         <v>514.28571428571422</v>
       </c>
       <c r="B8" s="5"/>
@@ -4924,7 +5238,7 @@
     </row>
     <row r="9" spans="1:15" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="31">
-        <f>A8+O$2</f>
+        <f t="shared" si="1"/>
         <v>599.99999999999989</v>
       </c>
       <c r="B9" s="5"/>
@@ -5027,151 +5341,151 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f t="shared" ref="A14:A25" si="0">IF(A13=6,0,A13+F$12)</f>
+        <f t="shared" ref="A14:A25" si="2">IF(A13=6,0,A13+F$12)</f>
         <v>1</v>
       </c>
       <c r="B14">
-        <f t="shared" ref="B14:B21" si="1">IF(A13=6,B13+H$12,B13)</f>
+        <f t="shared" ref="B14:B21" si="3">IF(A13=6,B13+H$12,B13)</f>
         <v>1</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:C21" si="2">O$5 + 1.5*L$5*COS(A14)*B14</f>
+        <f t="shared" ref="C14:C21" si="4">O$5 + 1.5*L$5*COS(A14)*B14</f>
         <v>606.90896672025258</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D14:D21" si="3">O$6+1.5*L$6*SIN(A14)*B14</f>
+        <f t="shared" ref="D14:D21" si="5">O$6+1.5*L$6*SIN(A14)*B14</f>
         <v>493.90341233244379</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
       <c r="B15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>526.41209171446337</v>
       </c>
       <c r="D15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>513.96364113480695</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="B16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>442.94625659191848</v>
       </c>
       <c r="D16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>502.62395487758761</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
       <c r="B17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>376.94680876338282</v>
       </c>
       <c r="D17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>462.6607042419372</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="B18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>344.5727148684951</v>
       </c>
       <c r="D18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>403.85828675055433</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
       <c r="B19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>353.75028217872068</v>
       </c>
       <c r="D19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>340.61358501133452</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="B20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>402.23252213766659</v>
       </c>
       <c r="D20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>288.41110774612349</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4.5</v>
       </c>
       <c r="B21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>478.14929152615207</v>
       </c>
       <c r="D21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>260.03184201448749</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="B22">
@@ -5189,43 +5503,43 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.5</v>
       </c>
       <c r="B23">
-        <f t="shared" ref="B23:B24" si="4">IF(A22=6,B22+H$12,B22)</f>
+        <f t="shared" ref="B23:B24" si="6">IF(A22=6,B22+H$12,B22)</f>
         <v>1</v>
       </c>
       <c r="C23">
-        <f t="shared" ref="C23:C24" si="5">O$5 + 1.5*L$5*COS(A23)*B23</f>
+        <f t="shared" ref="C23:C24" si="7">O$5 + 1.5*L$5*COS(A23)*B23</f>
         <v>635.77196130707318</v>
       </c>
       <c r="D23">
-        <f t="shared" ref="D23:D24" si="6">O$6+1.5*L$6*SIN(A23)*B23</f>
+        <f t="shared" ref="D23:D24" si="8">O$6+1.5*L$6*SIN(A23)*B23</f>
         <v>295.00195814094957</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="B24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="C24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>678.88633485434855</v>
       </c>
       <c r="D24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>349.78943594585235</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="B25">
@@ -5243,205 +5557,205 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
-        <f t="shared" ref="A26:A37" si="7">IF(A25=6,0,A25+F$12)</f>
+        <f t="shared" ref="A26:A37" si="9">IF(A25=6,0,A25+F$12)</f>
         <v>0.5</v>
       </c>
       <c r="B26">
-        <f t="shared" ref="B26:B36" si="8">IF(A25=6,B25+H$12,B25)</f>
+        <f t="shared" ref="B26:B36" si="10">IF(A25=6,B25+H$12,B25)</f>
         <v>1.5</v>
       </c>
       <c r="C26">
-        <f t="shared" ref="C26:C36" si="9">O$5 + 1.5*L$5*COS(A26)*B26</f>
+        <f t="shared" ref="C26:C36" si="11">O$5 + 1.5*L$5*COS(A26)*B26</f>
         <v>739.94980162895308</v>
       </c>
       <c r="D26">
-        <f t="shared" ref="D26:D36" si="10">O$6+1.5*L$6*SIN(A26)*B26</f>
+        <f t="shared" ref="D26:D36" si="12">O$6+1.5*L$6*SIN(A26)*B26</f>
         <v>478.1749253022391</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="B27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.5</v>
       </c>
       <c r="C27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>653.2205929375217</v>
       </c>
       <c r="D27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>547.99797564152277</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.5</v>
       </c>
       <c r="B28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.5</v>
       </c>
       <c r="C28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>532.47528042883789</v>
       </c>
       <c r="D28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>578.08831884506753</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="B29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.5</v>
       </c>
       <c r="C29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>407.27652774502053</v>
       </c>
       <c r="D29">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>561.07878945923858</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.5</v>
       </c>
       <c r="B30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.5</v>
       </c>
       <c r="C30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>308.27735600221706</v>
       </c>
       <c r="D30">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>501.13391350576296</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="B31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.5</v>
       </c>
       <c r="C31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>259.71621515988545</v>
       </c>
       <c r="D31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>412.93028726868863</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3.5</v>
       </c>
       <c r="B32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.5</v>
       </c>
       <c r="C32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>273.4825661252238</v>
       </c>
       <c r="D32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>318.06323465985901</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.5</v>
       </c>
       <c r="C33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>346.20592606364266</v>
       </c>
       <c r="D33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>239.75951876204238</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4.5</v>
       </c>
       <c r="B34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.5</v>
       </c>
       <c r="C34">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>460.08108014637099</v>
       </c>
       <c r="D34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>197.19062016458841</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="B35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.5</v>
       </c>
       <c r="C35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>587.22741911911544</v>
       </c>
       <c r="D35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>200.77888988639469</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5.5</v>
       </c>
       <c r="B36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.5</v>
       </c>
       <c r="C36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>696.51508481775261</v>
       </c>
       <c r="D36">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>249.64579435428152</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="B37">
@@ -5459,235 +5773,235 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
-        <f t="shared" ref="A38:A52" si="11">IF(A37=6,0,A37+F$12)</f>
+        <f t="shared" ref="A38:A50" si="13">IF(A37=6,0,A37+F$12)</f>
         <v>0</v>
       </c>
       <c r="B38">
-        <f t="shared" ref="B38:B52" si="12">IF(A37=6,B37+H$12,B37)</f>
+        <f t="shared" ref="B38:B50" si="14">IF(A37=6,B37+H$12,B37)</f>
         <v>2</v>
       </c>
       <c r="C38">
-        <f t="shared" ref="C38:C52" si="13">O$5 + 1.5*L$5*COS(A38)*B38</f>
+        <f t="shared" ref="C38:C50" si="15">O$5 + 1.5*L$5*COS(A38)*B38</f>
         <v>857.14285714285722</v>
       </c>
       <c r="D38">
-        <f t="shared" ref="D38:D52" si="14">O$6+1.5*L$6*SIN(A38)*B38</f>
+        <f t="shared" ref="D38:D50" si="16">O$6+1.5*L$6*SIN(A38)*B38</f>
         <v>385.71428571428567</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.5</v>
       </c>
       <c r="B39">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="C39">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>815.17116407669937</v>
       </c>
       <c r="D39">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>508.99513849822358</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="B40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="C40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>699.53221915479082</v>
       </c>
       <c r="D40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>602.09253895060192</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.5</v>
       </c>
       <c r="B41">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="C41">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>538.53846914321252</v>
       </c>
       <c r="D41">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>642.21299655532823</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="B42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="C42">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>371.60679889812263</v>
       </c>
       <c r="D42">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>619.53362404088944</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2.5</v>
       </c>
       <c r="B43">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="C43">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>239.6079032410513</v>
       </c>
       <c r="D43">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>539.60712276958873</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
       <c r="B44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="C44">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>174.85971545127586</v>
       </c>
       <c r="D44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>422.00228778682293</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.5</v>
       </c>
       <c r="B45">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="C45">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>193.21485007172697</v>
       </c>
       <c r="D45">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>295.51288430838343</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>4</v>
       </c>
       <c r="B46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="C46">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>290.17932998961879</v>
       </c>
       <c r="D46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>191.10792977796129</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>4.5</v>
       </c>
       <c r="B47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="C47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>442.01286876658986</v>
       </c>
       <c r="D47">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>134.34939831468932</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5</v>
       </c>
       <c r="B48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="C48">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>611.54132073024903</v>
       </c>
       <c r="D48">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>139.13375794376438</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5.5</v>
       </c>
       <c r="B49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="C49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>757.25820832843203</v>
       </c>
       <c r="D49">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>204.28963056761347</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>6</v>
       </c>
       <c r="B50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="C50">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>843.48695542298265</v>
       </c>
       <c r="D50">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>313.86458617741903</v>
       </c>
     </row>
@@ -5696,4 +6010,269 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <f>E2</f>
+        <v>114</v>
+      </c>
+      <c r="B2">
+        <f>E3</f>
+        <v>425</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>E2</f>
+        <v>114</v>
+      </c>
+      <c r="B3">
+        <f>E3+E5</f>
+        <v>510</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f>E2+E4</f>
+        <v>228</v>
+      </c>
+      <c r="B4">
+        <f>E3+E5</f>
+        <v>510</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f>E2+E4</f>
+        <v>228</v>
+      </c>
+      <c r="B5">
+        <f>E3</f>
+        <v>425</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f>E2</f>
+        <v>114</v>
+      </c>
+      <c r="B6">
+        <f>E3</f>
+        <v>425</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f>E8</f>
+        <v>56</v>
+      </c>
+      <c r="B8">
+        <f>E9</f>
+        <v>510</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f>E8</f>
+        <v>56</v>
+      </c>
+      <c r="B9">
+        <f>E9+E11</f>
+        <v>552</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f>E8+E10</f>
+        <v>113</v>
+      </c>
+      <c r="B10">
+        <f>E9+E11</f>
+        <v>552</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f>E8+E10</f>
+        <v>113</v>
+      </c>
+      <c r="B11">
+        <f>E9</f>
+        <v>510</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f>E8</f>
+        <v>56</v>
+      </c>
+      <c r="B12">
+        <f>E9</f>
+        <v>510</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f>E14</f>
+        <v>61</v>
+      </c>
+      <c r="B14">
+        <f>E15</f>
+        <v>510</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f>E14</f>
+        <v>61</v>
+      </c>
+      <c r="B15">
+        <f>E15+E17</f>
+        <v>552</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f>E14+E16</f>
+        <v>118</v>
+      </c>
+      <c r="B16">
+        <f>E15+E17</f>
+        <v>552</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f>E14+E16</f>
+        <v>118</v>
+      </c>
+      <c r="B17">
+        <f>E15</f>
+        <v>510</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f>E14</f>
+        <v>61</v>
+      </c>
+      <c r="B18">
+        <f>E15</f>
+        <v>510</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Oh no! Monsters can attack Zero but he can't fight back!
Luckily, game over screen hasn't developed yet.
Now each playing object has life bar over it. As introduced - if Zero is in touch with any monster then they attack it with certain speed and Zero's life bar decreases until it reach to 0. Nothing else happens though.
Some minor refactorings made.
Some wishes in the todo list.
</commit_message>
<xml_diff>
--- a/calcs.xlsx
+++ b/calcs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8136" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8136" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="frames" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="scaleSpriteTo" sheetId="8" r:id="rId7"/>
     <sheet name="monsters" sheetId="9" r:id="rId8"/>
     <sheet name="process collisions 2" sheetId="10" r:id="rId9"/>
+    <sheet name="health" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="152">
   <si>
     <t>y \ x</t>
   </si>
@@ -583,12 +584,51 @@
   <si>
     <t>monster now</t>
   </si>
+  <si>
+    <t>health</t>
+  </si>
+  <si>
+    <t>newWidth</t>
+  </si>
+  <si>
+    <t>m_maxWidth - m_maxWidth * (m_currentHealth / m_maxHealth)</t>
+  </si>
+  <si>
+    <t>maxWidth</t>
+  </si>
+  <si>
+    <t>maxHealth</t>
+  </si>
+  <si>
+    <t>currentHealth</t>
+  </si>
+  <si>
+    <t>gameObject</t>
+  </si>
+  <si>
+    <t>scale health bar</t>
+  </si>
+  <si>
+    <t>m_maxWidth</t>
+  </si>
+  <si>
+    <t>texture.x</t>
+  </si>
+  <si>
+    <t>factor1</t>
+  </si>
+  <si>
+    <t>newWidth * frames / texture.x</t>
+  </si>
+  <si>
+    <t>sprite.scale.x</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -631,8 +671,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -693,8 +742,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -797,11 +851,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -863,8 +933,10 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -1008,11 +1080,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="275059456"/>
-        <c:axId val="275060992"/>
+        <c:axId val="281699840"/>
+        <c:axId val="281701376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="275059456"/>
+        <c:axId val="281699840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="800"/>
@@ -1023,13 +1095,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="275060992"/>
+        <c:crossAx val="281701376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="275060992"/>
+        <c:axId val="281701376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1040,7 +1112,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="275059456"/>
+        <c:crossAx val="281699840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1072,7 +1144,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1366,11 +1437,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="275746816"/>
-        <c:axId val="275748352"/>
+        <c:axId val="276427520"/>
+        <c:axId val="276429056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="275746816"/>
+        <c:axId val="276427520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1381,13 +1452,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="275748352"/>
+        <c:crossAx val="276429056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="114"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="275748352"/>
+        <c:axId val="276429056"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1398,7 +1469,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="275746816"/>
+        <c:crossAx val="276427520"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="85"/>
@@ -1636,11 +1707,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="43809024"/>
-        <c:axId val="43807488"/>
+        <c:axId val="276480000"/>
+        <c:axId val="276481536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43809024"/>
+        <c:axId val="276480000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1650,12 +1721,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43807488"/>
+        <c:crossAx val="276481536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43807488"/>
+        <c:axId val="276481536"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1666,14 +1737,130 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43809024"/>
+        <c:crossAx val="276480000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
       <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>health!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>gameObject</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>health</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>health!$B$2:$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="276788736"/>
+        <c:axId val="276790272"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="276788736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="276790272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="276790272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="276788736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2474,6 +2661,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема на Office">
   <a:themeElements>
@@ -3112,6 +3334,136 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3">
+        <f>B2/D1</f>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17">
+        <f>B14*(B16/B15)</f>
+        <v>54.15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:3" s="35" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="35" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23">
+        <v>54.149999999999899</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>148</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>149</v>
+      </c>
+      <c r="B25">
+        <f>B23*1/B24</f>
+        <v>18.049999999999965</v>
+      </c>
+      <c r="C25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
@@ -6016,7 +6368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Zero's firing logic completed
1. Refined the arrow's image
2. Added to the Zero's data file his attacking speed and initial firing accurracy
3. Refined the attacking logic for the playing objects (Zero or Monsters) in a way that the attack starts immediately but not when the attacking speed time has elapsed.
4. Don't set as inactive Zero (for now) as the way the other playing objects are - later there the game over event to be raised
5. The projectiles are rotated to the direction they are moving to
6. Added inaccuracy to the Zero's firing skills - for
</commit_message>
<xml_diff>
--- a/calcs.xlsx
+++ b/calcs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8136" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8136" firstSheet="4" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="frames" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="process collisions 2" sheetId="10" r:id="rId9"/>
     <sheet name="health" sheetId="11" r:id="rId10"/>
     <sheet name="projectiles movement" sheetId="12" r:id="rId11"/>
+    <sheet name="firing accuracy" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="165">
   <si>
     <t>y \ x</t>
   </si>
@@ -641,6 +642,27 @@
   </si>
   <si>
     <t>new m_rect</t>
+  </si>
+  <si>
+    <t>m_firingAccuracy</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>error range</t>
+  </si>
+  <si>
+    <t>rand</t>
+  </si>
+  <si>
+    <t>inaccuracy</t>
+  </si>
+  <si>
+    <t>100 - firingAccuracy</t>
+  </si>
+  <si>
+    <t>rand - errorRange / 2</t>
   </si>
 </sst>
 </file>
@@ -1099,11 +1121,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="153000192"/>
-        <c:axId val="153022464"/>
+        <c:axId val="300180608"/>
+        <c:axId val="300182912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="153000192"/>
+        <c:axId val="300180608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="800"/>
@@ -1114,13 +1136,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153022464"/>
+        <c:crossAx val="300182912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="153022464"/>
+        <c:axId val="300182912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1131,7 +1153,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153000192"/>
+        <c:crossAx val="300180608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1456,11 +1478,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="153466368"/>
-        <c:axId val="153467904"/>
+        <c:axId val="292550144"/>
+        <c:axId val="292551680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="153466368"/>
+        <c:axId val="292550144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1471,13 +1493,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153467904"/>
+        <c:crossAx val="292551680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="114"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="153467904"/>
+        <c:axId val="292551680"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1488,7 +1510,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153466368"/>
+        <c:crossAx val="292550144"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="85"/>
@@ -1726,11 +1748,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="153236224"/>
-        <c:axId val="153237760"/>
+        <c:axId val="291922688"/>
+        <c:axId val="291924224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="153236224"/>
+        <c:axId val="291922688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1740,12 +1762,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153237760"/>
+        <c:crossAx val="291924224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="153237760"/>
+        <c:axId val="291924224"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1756,7 +1778,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153236224"/>
+        <c:crossAx val="291922688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1841,11 +1863,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153557248"/>
-        <c:axId val="153575424"/>
+        <c:axId val="292720640"/>
+        <c:axId val="292722176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153557248"/>
+        <c:axId val="292720640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1854,7 +1876,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153575424"/>
+        <c:crossAx val="292722176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1862,7 +1884,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153575424"/>
+        <c:axId val="292722176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1873,7 +1895,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153557248"/>
+        <c:crossAx val="292720640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1977,11 +1999,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="37403648"/>
-        <c:axId val="37402112"/>
+        <c:axId val="292955648"/>
+        <c:axId val="292957184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="37403648"/>
+        <c:axId val="292955648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1991,12 +2013,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37402112"/>
+        <c:crossAx val="292957184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="37402112"/>
+        <c:axId val="292957184"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2007,7 +2029,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37403648"/>
+        <c:crossAx val="292955648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3140,7 +3162,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3657,7 +3679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -3744,6 +3766,71 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3">
+        <f>100-B2</f>
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4">
+        <f ca="1">RANDBETWEEN(0,B3)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5">
+        <f ca="1">B4-B3/2</f>
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Optimized game constants - speeds, healths, damages, etc.
</commit_message>
<xml_diff>
--- a/calcs.xlsx
+++ b/calcs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8136" firstSheet="4" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8136" firstSheet="6" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="frames" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="health" sheetId="11" r:id="rId10"/>
     <sheet name="projectiles movement" sheetId="12" r:id="rId11"/>
     <sheet name="firing accuracy" sheetId="13" r:id="rId12"/>
+    <sheet name="balance game consts" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="179">
   <si>
     <t>y \ x</t>
   </si>
@@ -664,17 +665,67 @@
   <si>
     <t>rand - errorRange / 2</t>
   </si>
+  <si>
+    <t>nameOfTexture</t>
+  </si>
+  <si>
+    <t>rowsForAnimation</t>
+  </si>
+  <si>
+    <t>columnsForAnimation</t>
+  </si>
+  <si>
+    <t>attackRate</t>
+  </si>
+  <si>
+    <t>minDamage</t>
+  </si>
+  <si>
+    <t>maxDamage</t>
+  </si>
+  <si>
+    <t>attackRange</t>
+  </si>
+  <si>
+    <t>resistentToProjectiles)</t>
+  </si>
+  <si>
+    <t>monsterSpriteSheet"</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Jelly"</t>
+  </si>
+  <si>
+    <t>1.5f</t>
+  </si>
+  <si>
+    <t>WalkingSquare"</t>
+  </si>
+  <si>
+    <t>creatureResistentToProjectiles</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -910,9 +961,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -930,16 +981,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -950,20 +1001,20 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -974,7 +1025,10 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="10" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -1121,11 +1175,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="300180608"/>
-        <c:axId val="300182912"/>
+        <c:axId val="278888832"/>
+        <c:axId val="278890368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="300180608"/>
+        <c:axId val="278888832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="800"/>
@@ -1136,13 +1190,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="300182912"/>
+        <c:crossAx val="278890368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="300182912"/>
+        <c:axId val="278890368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1153,7 +1207,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="300180608"/>
+        <c:crossAx val="278888832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1478,11 +1532,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="292550144"/>
-        <c:axId val="292551680"/>
+        <c:axId val="279457152"/>
+        <c:axId val="279458944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="292550144"/>
+        <c:axId val="279457152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1493,13 +1547,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="292551680"/>
+        <c:crossAx val="279458944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="114"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="292551680"/>
+        <c:axId val="279458944"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1510,7 +1564,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="292550144"/>
+        <c:crossAx val="279457152"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="85"/>
@@ -1748,11 +1802,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="291922688"/>
-        <c:axId val="291924224"/>
+        <c:axId val="279480960"/>
+        <c:axId val="279490944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="291922688"/>
+        <c:axId val="279480960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1762,12 +1816,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="291924224"/>
+        <c:crossAx val="279490944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="291924224"/>
+        <c:axId val="279490944"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1778,7 +1832,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="291922688"/>
+        <c:crossAx val="279480960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1863,11 +1917,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="292720640"/>
-        <c:axId val="292722176"/>
+        <c:axId val="279816064"/>
+        <c:axId val="279817600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="292720640"/>
+        <c:axId val="279816064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1876,7 +1930,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="292722176"/>
+        <c:crossAx val="279817600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1884,7 +1938,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292722176"/>
+        <c:axId val="279817600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1895,7 +1949,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="292720640"/>
+        <c:crossAx val="279816064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1931,7 +1985,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1999,11 +2052,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="292955648"/>
-        <c:axId val="292957184"/>
+        <c:axId val="279990272"/>
+        <c:axId val="279991808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="292955648"/>
+        <c:axId val="279990272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2013,12 +2066,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="292957184"/>
+        <c:crossAx val="279991808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="292957184"/>
+        <c:axId val="279991808"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2029,14 +2082,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="292955648"/>
+        <c:crossAx val="279990272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3162,7 +3214,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3773,7 +3825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -3814,7 +3866,7 @@
       </c>
       <c r="B4">
         <f ca="1">RANDBETWEEN(0,B3)</f>
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3823,7 +3875,7 @@
       </c>
       <c r="B5">
         <f ca="1">B4-B3/2</f>
-        <v>4</v>
+        <v>-12</v>
       </c>
       <c r="D5" t="s">
         <v>164</v>
@@ -3831,6 +3883,175 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.109375" customWidth="1"/>
+    <col min="3" max="3" width="3.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>171</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="36">
+        <v>1</v>
+      </c>
+      <c r="C2" s="36">
+        <v>7</v>
+      </c>
+      <c r="D2" s="36">
+        <v>50</v>
+      </c>
+      <c r="E2" s="36">
+        <v>3</v>
+      </c>
+      <c r="F2" s="36">
+        <v>100</v>
+      </c>
+      <c r="G2" s="36">
+        <v>2000</v>
+      </c>
+      <c r="H2" s="36">
+        <v>10</v>
+      </c>
+      <c r="I2" s="36">
+        <v>1</v>
+      </c>
+      <c r="J2" s="36">
+        <v>1</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="36">
+        <v>2</v>
+      </c>
+      <c r="C3" s="36">
+        <v>2</v>
+      </c>
+      <c r="D3" s="36">
+        <v>70</v>
+      </c>
+      <c r="E3" s="36">
+        <v>1</v>
+      </c>
+      <c r="F3" s="36">
+        <v>100</v>
+      </c>
+      <c r="G3" s="36">
+        <v>1000</v>
+      </c>
+      <c r="H3" s="36">
+        <v>20</v>
+      </c>
+      <c r="I3" s="36">
+        <v>1</v>
+      </c>
+      <c r="J3" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="K3" s="36" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="36" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" s="36">
+        <v>1</v>
+      </c>
+      <c r="C4" s="36">
+        <v>5</v>
+      </c>
+      <c r="D4" s="36">
+        <v>150</v>
+      </c>
+      <c r="E4" s="36">
+        <v>2</v>
+      </c>
+      <c r="F4" s="36">
+        <v>300</v>
+      </c>
+      <c r="G4" s="36">
+        <v>1000</v>
+      </c>
+      <c r="H4" s="36">
+        <v>100</v>
+      </c>
+      <c r="I4" s="36">
+        <v>1</v>
+      </c>
+      <c r="J4" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="K4" s="36" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Speed of objects depends of the size of the objects (smaller objects -> smaller speed)
</commit_message>
<xml_diff>
--- a/calcs.xlsx
+++ b/calcs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8136" firstSheet="6" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8136" firstSheet="7" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="frames" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="projectiles movement" sheetId="12" r:id="rId11"/>
     <sheet name="firing accuracy" sheetId="13" r:id="rId12"/>
     <sheet name="balance game consts" sheetId="14" r:id="rId13"/>
+    <sheet name="objs speed" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="188">
   <si>
     <t>y \ x</t>
   </si>
@@ -706,6 +707,33 @@
   </si>
   <si>
     <t>creatureResistentToProjectiles</t>
+  </si>
+  <si>
+    <t>screen_x</t>
+  </si>
+  <si>
+    <t>screen_y</t>
+  </si>
+  <si>
+    <t>blocks_x</t>
+  </si>
+  <si>
+    <t>blocks_y</t>
+  </si>
+  <si>
+    <t>nblocks_x</t>
+  </si>
+  <si>
+    <t>nblocks_y</t>
+  </si>
+  <si>
+    <t>speedFactor</t>
+  </si>
+  <si>
+    <t>speed pixels</t>
+  </si>
+  <si>
+    <t>divider</t>
   </si>
 </sst>
 </file>
@@ -1175,11 +1203,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="278888832"/>
-        <c:axId val="278890368"/>
+        <c:axId val="271050624"/>
+        <c:axId val="284295552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="278888832"/>
+        <c:axId val="271050624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="800"/>
@@ -1190,13 +1218,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="278890368"/>
+        <c:crossAx val="284295552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="278890368"/>
+        <c:axId val="284295552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1207,7 +1235,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="278888832"/>
+        <c:crossAx val="271050624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1532,11 +1560,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="279457152"/>
-        <c:axId val="279458944"/>
+        <c:axId val="266641408"/>
+        <c:axId val="266642944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="279457152"/>
+        <c:axId val="266641408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1547,13 +1575,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="279458944"/>
+        <c:crossAx val="266642944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="114"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="279458944"/>
+        <c:axId val="266642944"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1564,7 +1592,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="279457152"/>
+        <c:crossAx val="266641408"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="85"/>
@@ -1802,11 +1830,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="279480960"/>
-        <c:axId val="279490944"/>
+        <c:axId val="266476544"/>
+        <c:axId val="266478336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="279480960"/>
+        <c:axId val="266476544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1816,12 +1844,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="279490944"/>
+        <c:crossAx val="266478336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="279490944"/>
+        <c:axId val="266478336"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1832,7 +1860,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="279480960"/>
+        <c:crossAx val="266476544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1917,11 +1945,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="279816064"/>
-        <c:axId val="279817600"/>
+        <c:axId val="267342592"/>
+        <c:axId val="267344128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="279816064"/>
+        <c:axId val="267342592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1930,7 +1958,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="279817600"/>
+        <c:crossAx val="267344128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1938,7 +1966,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="279817600"/>
+        <c:axId val="267344128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1949,7 +1977,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="279816064"/>
+        <c:crossAx val="267342592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2052,11 +2080,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="279990272"/>
-        <c:axId val="279991808"/>
+        <c:axId val="267374592"/>
+        <c:axId val="267376128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="279990272"/>
+        <c:axId val="267374592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2066,12 +2094,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="279991808"/>
+        <c:crossAx val="267376128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="279991808"/>
+        <c:axId val="267376128"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2082,7 +2110,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="279990272"/>
+        <c:crossAx val="267374592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3214,7 +3242,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3866,7 +3894,7 @@
       </c>
       <c r="B4">
         <f ca="1">RANDBETWEEN(0,B3)</f>
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3875,7 +3903,7 @@
       </c>
       <c r="B5">
         <f ca="1">B4-B3/2</f>
-        <v>-12</v>
+        <v>-3</v>
       </c>
       <c r="D5" t="s">
         <v>164</v>
@@ -3890,7 +3918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -4052,6 +4080,377 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="15" width="7.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1">
+        <v>10</v>
+      </c>
+      <c r="F1">
+        <v>1</v>
+      </c>
+      <c r="G1">
+        <v>2</v>
+      </c>
+      <c r="H1">
+        <v>3</v>
+      </c>
+      <c r="I1">
+        <v>4</v>
+      </c>
+      <c r="J1">
+        <v>5</v>
+      </c>
+      <c r="K1">
+        <v>6</v>
+      </c>
+      <c r="L1">
+        <v>7</v>
+      </c>
+      <c r="M1">
+        <v>8</v>
+      </c>
+      <c r="N1">
+        <v>9</v>
+      </c>
+      <c r="O1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2">
+        <v>640</v>
+      </c>
+      <c r="F2">
+        <f>$B6*F1</f>
+        <v>64</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:O2" si="0">$B6*G1</f>
+        <v>128</v>
+      </c>
+      <c r="H2">
+        <f t="shared" si="0"/>
+        <v>192</v>
+      </c>
+      <c r="I2">
+        <f t="shared" si="0"/>
+        <v>256</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="0"/>
+        <v>320</v>
+      </c>
+      <c r="K2">
+        <f t="shared" si="0"/>
+        <v>384</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="0"/>
+        <v>448</v>
+      </c>
+      <c r="M2">
+        <f t="shared" si="0"/>
+        <v>512</v>
+      </c>
+      <c r="N2">
+        <f t="shared" si="0"/>
+        <v>576</v>
+      </c>
+      <c r="O2">
+        <f t="shared" si="0"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3">
+        <v>480</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f>B$7*D3</f>
+        <v>48</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+    </row>
+    <row r="4" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E12" si="1">B$7*D4</f>
+        <v>96</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+    </row>
+    <row r="5" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>144</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B6">
+        <f>B2/B4</f>
+        <v>64</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>192</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7">
+        <f>B3/B5</f>
+        <v>48</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>288</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>336</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+    </row>
+    <row r="10" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <f>B6/B$9</f>
+        <v>0.64</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>384</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f>B7/B$9</f>
+        <v>0.48</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>432</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>480</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <f>B$1*B10</f>
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <f>B$1*B11</f>
+        <v>4.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Monsters looking for Zero at not so precise way (but still enough) so the game speed is not affected so much
</commit_message>
<xml_diff>
--- a/calcs.xlsx
+++ b/calcs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8136" firstSheet="7" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8136" firstSheet="7" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="frames" sheetId="1" r:id="rId1"/>
@@ -858,13 +858,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -989,9 +989,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1046,16 +1046,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="10" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="10" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1203,11 +1200,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="271050624"/>
-        <c:axId val="284295552"/>
+        <c:axId val="265452928"/>
+        <c:axId val="265753728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="271050624"/>
+        <c:axId val="265452928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="800"/>
@@ -1218,13 +1215,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="284295552"/>
+        <c:crossAx val="265753728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="284295552"/>
+        <c:axId val="265753728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1235,7 +1232,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="271050624"/>
+        <c:crossAx val="265452928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1267,6 +1264,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1305,121 +1303,121 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
-                  <c:v>685.71428571428578</c:v>
+                  <c:v>621.42857142857144</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>664.7284391812068</c:v>
+                  <c:v>600.44272489549246</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>606.90896672025258</c:v>
+                  <c:v>542.62325243453824</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>526.41209171446337</c:v>
+                  <c:v>462.12637742874909</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>442.94625659191848</c:v>
+                  <c:v>378.66054230620415</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>376.94680876338282</c:v>
+                  <c:v>312.66109447766848</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>344.5727148684951</c:v>
+                  <c:v>280.28700058278076</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>353.75028217872068</c:v>
+                  <c:v>289.46456789300635</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>402.23252213766659</c:v>
+                  <c:v>337.94680785195226</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>478.14929152615207</c:v>
+                  <c:v>413.86357724043773</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>562.91351750798174</c:v>
+                  <c:v>498.62780322226735</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>635.77196130707318</c:v>
+                  <c:v>571.48624702135885</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>678.88633485434855</c:v>
+                  <c:v>614.60062056863421</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>771.42857142857156</c:v>
+                  <c:v>707.14285714285711</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>739.94980162895308</c:v>
+                  <c:v>675.66408734323875</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>653.2205929375217</c:v>
+                  <c:v>588.93487865180737</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>532.47528042883789</c:v>
+                  <c:v>468.18956614312361</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>407.27652774502053</c:v>
+                  <c:v>342.9908134593062</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>308.27735600221706</c:v>
+                  <c:v>243.99164171650273</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>259.71621515988545</c:v>
+                  <c:v>195.43050087417114</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>273.4825661252238</c:v>
+                  <c:v>209.19685183950946</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>346.20592606364266</c:v>
+                  <c:v>281.92021177792833</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>460.08108014637099</c:v>
+                  <c:v>395.79536586065666</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>587.22741911911544</c:v>
+                  <c:v>522.94170483340099</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>696.51508481775261</c:v>
+                  <c:v>632.22937053203827</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>761.18664513866565</c:v>
+                  <c:v>696.90093085295121</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>857.14285714285722</c:v>
+                  <c:v>792.85714285714289</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>815.17116407669937</c:v>
+                  <c:v>750.88544979098492</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>699.53221915479082</c:v>
+                  <c:v>635.24650486907649</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>538.53846914321252</c:v>
+                  <c:v>474.25275485749813</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>371.60679889812263</c:v>
+                  <c:v>307.3210846124083</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>239.6079032410513</c:v>
+                  <c:v>175.32218895533697</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>174.85971545127586</c:v>
+                  <c:v>110.57400116556153</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>193.21485007172697</c:v>
+                  <c:v>128.92913578601264</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>290.17932998961879</c:v>
+                  <c:v>225.89361570390446</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>442.01286876658986</c:v>
+                  <c:v>377.72715448087553</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>611.54132073024903</c:v>
+                  <c:v>547.25560644453469</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>757.25820832843203</c:v>
+                  <c:v>692.9724940427177</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>843.48695542298265</c:v>
+                  <c:v>779.20124113726843</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1560,11 +1558,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="266641408"/>
-        <c:axId val="266642944"/>
+        <c:axId val="266369664"/>
+        <c:axId val="266371456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="266641408"/>
+        <c:axId val="266369664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1575,13 +1573,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266642944"/>
+        <c:crossAx val="266371456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="114"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="266642944"/>
+        <c:axId val="266371456"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1592,7 +1590,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266641408"/>
+        <c:crossAx val="266369664"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="85"/>
@@ -1830,11 +1828,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="266476544"/>
-        <c:axId val="266478336"/>
+        <c:axId val="266635136"/>
+        <c:axId val="266636672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="266476544"/>
+        <c:axId val="266635136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1844,12 +1842,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266478336"/>
+        <c:crossAx val="266636672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="266478336"/>
+        <c:axId val="266636672"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1860,7 +1858,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266476544"/>
+        <c:crossAx val="266635136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1945,11 +1943,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="267342592"/>
-        <c:axId val="267344128"/>
+        <c:axId val="266542464"/>
+        <c:axId val="266552448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="267342592"/>
+        <c:axId val="266542464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1958,7 +1956,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="267344128"/>
+        <c:crossAx val="266552448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1966,7 +1964,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="267344128"/>
+        <c:axId val="266552448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1977,7 +1975,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="267342592"/>
+        <c:crossAx val="266542464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2080,11 +2078,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="267374592"/>
-        <c:axId val="267376128"/>
+        <c:axId val="266803840"/>
+        <c:axId val="266817920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="267374592"/>
+        <c:axId val="266803840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2094,12 +2092,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="267376128"/>
+        <c:crossAx val="266817920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="267376128"/>
+        <c:axId val="266817920"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2110,7 +2108,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="267374592"/>
+        <c:crossAx val="266803840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3242,7 +3240,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3700,8 +3698,8 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="1:3" s="35" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="35" t="s">
+    <row r="21" spans="1:3" s="32" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="32" t="s">
         <v>146</v>
       </c>
     </row>
@@ -3894,7 +3892,7 @@
       </c>
       <c r="B4">
         <f ca="1">RANDBETWEEN(0,B3)</f>
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3903,7 +3901,7 @@
       </c>
       <c r="B5">
         <f ca="1">B4-B3/2</f>
-        <v>-3</v>
+        <v>-10</v>
       </c>
       <c r="D5" t="s">
         <v>164</v>
@@ -3938,142 +3936,142 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="33" t="s">
         <v>165</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="33" t="s">
         <v>166</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="33" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="33" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="36">
+      <c r="B2" s="33">
         <v>1</v>
       </c>
-      <c r="C2" s="36">
+      <c r="C2" s="33">
         <v>7</v>
       </c>
-      <c r="D2" s="36">
+      <c r="D2" s="33">
         <v>50</v>
       </c>
-      <c r="E2" s="36">
+      <c r="E2" s="33">
         <v>3</v>
       </c>
-      <c r="F2" s="36">
+      <c r="F2" s="33">
         <v>100</v>
       </c>
-      <c r="G2" s="36">
+      <c r="G2" s="33">
         <v>2000</v>
       </c>
-      <c r="H2" s="36">
+      <c r="H2" s="33">
         <v>10</v>
       </c>
-      <c r="I2" s="36">
+      <c r="I2" s="33">
         <v>1</v>
       </c>
-      <c r="J2" s="36">
+      <c r="J2" s="33">
         <v>1</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="33" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="B3" s="36">
+      <c r="B3" s="33">
         <v>2</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="33">
         <v>2</v>
       </c>
-      <c r="D3" s="36">
+      <c r="D3" s="33">
         <v>70</v>
       </c>
-      <c r="E3" s="36">
+      <c r="E3" s="33">
         <v>1</v>
       </c>
-      <c r="F3" s="36">
+      <c r="F3" s="33">
         <v>100</v>
       </c>
-      <c r="G3" s="36">
+      <c r="G3" s="33">
         <v>1000</v>
       </c>
-      <c r="H3" s="36">
+      <c r="H3" s="33">
         <v>20</v>
       </c>
-      <c r="I3" s="36">
+      <c r="I3" s="33">
         <v>1</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="J3" s="33" t="s">
         <v>176</v>
       </c>
-      <c r="K3" s="36" t="s">
+      <c r="K3" s="33" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="B4" s="36">
+      <c r="B4" s="33">
         <v>1</v>
       </c>
-      <c r="C4" s="36">
+      <c r="C4" s="33">
         <v>5</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="33">
         <v>150</v>
       </c>
-      <c r="E4" s="36">
+      <c r="E4" s="33">
         <v>2</v>
       </c>
-      <c r="F4" s="36">
+      <c r="F4" s="33">
         <v>300</v>
       </c>
-      <c r="G4" s="36">
+      <c r="G4" s="33">
         <v>1000</v>
       </c>
-      <c r="H4" s="36">
+      <c r="H4" s="33">
         <v>100</v>
       </c>
-      <c r="I4" s="36">
+      <c r="I4" s="33">
         <v>1</v>
       </c>
-      <c r="J4" s="36" t="s">
+      <c r="J4" s="33" t="s">
         <v>176</v>
       </c>
-      <c r="K4" s="36" t="s">
+      <c r="K4" s="33" t="s">
         <v>178</v>
       </c>
     </row>
@@ -4087,7 +4085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -6368,8 +6366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6403,32 +6401,31 @@
         <v>59</v>
       </c>
       <c r="B2" s="31">
-        <f>O1</f>
-        <v>114.28571428571429</v>
+        <v>50</v>
       </c>
       <c r="C2" s="31">
         <f t="shared" ref="C2:H2" si="0">B2+$O1</f>
-        <v>228.57142857142858</v>
+        <v>164.28571428571428</v>
       </c>
       <c r="D2" s="31">
         <f t="shared" si="0"/>
-        <v>342.85714285714289</v>
+        <v>278.57142857142856</v>
       </c>
       <c r="E2" s="31">
         <f t="shared" si="0"/>
-        <v>457.14285714285717</v>
+        <v>392.85714285714283</v>
       </c>
       <c r="F2" s="31">
         <f t="shared" si="0"/>
-        <v>571.42857142857144</v>
+        <v>507.14285714285711</v>
       </c>
       <c r="G2" s="31">
         <f t="shared" si="0"/>
-        <v>685.71428571428578</v>
+        <v>621.42857142857144</v>
       </c>
       <c r="H2" s="31">
         <f t="shared" si="0"/>
-        <v>800.00000000000011</v>
+        <v>735.71428571428578</v>
       </c>
       <c r="K2" t="s">
         <v>119</v>
@@ -6461,7 +6458,7 @@
       </c>
       <c r="L3" s="31">
         <f>E2</f>
-        <v>457.14285714285717</v>
+        <v>392.85714285714283</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -6470,12 +6467,12 @@
         <v>171.42857142857142</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
       <c r="K4" t="s">
         <v>122</v>
       </c>
@@ -6490,12 +6487,12 @@
         <v>257.14285714285711</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
       <c r="K5" t="s">
         <v>123</v>
       </c>
@@ -6508,7 +6505,7 @@
       </c>
       <c r="O5">
         <f>L3+(L5/2)</f>
-        <v>514.28571428571433</v>
+        <v>450</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -6517,12 +6514,12 @@
         <v>342.85714285714283</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
       <c r="K6" t="s">
         <v>126</v>
       </c>
@@ -6544,14 +6541,14 @@
         <v>428.57142857142856</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="32" t="s">
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
       <c r="K7" t="s">
         <v>127</v>
       </c>
@@ -6565,12 +6562,12 @@
         <v>514.28571428571422</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
       <c r="K8" t="s">
         <v>128</v>
       </c>
@@ -6584,12 +6581,12 @@
         <v>599.99999999999989</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="5"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
       <c r="K9" t="s">
         <v>129</v>
       </c>
@@ -6631,7 +6628,7 @@
       </c>
       <c r="L11">
         <f>O5 + 1.5*L5*COS(L7)*L8</f>
-        <v>685.71428571428578</v>
+        <v>621.42857142857144</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -6643,7 +6640,7 @@
       </c>
       <c r="C12">
         <f>O$5 + 1.5*L$5*COS(A12)*B12</f>
-        <v>685.71428571428578</v>
+        <v>621.42857142857144</v>
       </c>
       <c r="D12">
         <f>O$6+1.5*L$6*SIN(A12)*B12</f>
@@ -6674,7 +6671,7 @@
       </c>
       <c r="C13">
         <f>O$5 + 1.5*L$5*COS(A13)*B13</f>
-        <v>664.7284391812068</v>
+        <v>600.44272489549246</v>
       </c>
       <c r="D13">
         <f>O$6+1.5*L$6*SIN(A13)*B13</f>
@@ -6692,7 +6689,7 @@
       </c>
       <c r="C14">
         <f t="shared" ref="C14:C21" si="4">O$5 + 1.5*L$5*COS(A14)*B14</f>
-        <v>606.90896672025258</v>
+        <v>542.62325243453824</v>
       </c>
       <c r="D14">
         <f t="shared" ref="D14:D21" si="5">O$6+1.5*L$6*SIN(A14)*B14</f>
@@ -6710,7 +6707,7 @@
       </c>
       <c r="C15">
         <f t="shared" si="4"/>
-        <v>526.41209171446337</v>
+        <v>462.12637742874909</v>
       </c>
       <c r="D15">
         <f t="shared" si="5"/>
@@ -6728,7 +6725,7 @@
       </c>
       <c r="C16">
         <f t="shared" si="4"/>
-        <v>442.94625659191848</v>
+        <v>378.66054230620415</v>
       </c>
       <c r="D16">
         <f t="shared" si="5"/>
@@ -6746,7 +6743,7 @@
       </c>
       <c r="C17">
         <f t="shared" si="4"/>
-        <v>376.94680876338282</v>
+        <v>312.66109447766848</v>
       </c>
       <c r="D17">
         <f t="shared" si="5"/>
@@ -6764,7 +6761,7 @@
       </c>
       <c r="C18">
         <f t="shared" si="4"/>
-        <v>344.5727148684951</v>
+        <v>280.28700058278076</v>
       </c>
       <c r="D18">
         <f t="shared" si="5"/>
@@ -6782,7 +6779,7 @@
       </c>
       <c r="C19">
         <f t="shared" si="4"/>
-        <v>353.75028217872068</v>
+        <v>289.46456789300635</v>
       </c>
       <c r="D19">
         <f t="shared" si="5"/>
@@ -6800,7 +6797,7 @@
       </c>
       <c r="C20">
         <f t="shared" si="4"/>
-        <v>402.23252213766659</v>
+        <v>337.94680785195226</v>
       </c>
       <c r="D20">
         <f t="shared" si="5"/>
@@ -6818,7 +6815,7 @@
       </c>
       <c r="C21">
         <f t="shared" si="4"/>
-        <v>478.14929152615207</v>
+        <v>413.86357724043773</v>
       </c>
       <c r="D21">
         <f t="shared" si="5"/>
@@ -6836,7 +6833,7 @@
       </c>
       <c r="C22">
         <f>O$5 + 1.5*L$5*COS(A22)*B22</f>
-        <v>562.91351750798174</v>
+        <v>498.62780322226735</v>
       </c>
       <c r="D22">
         <f>O$6+1.5*L$6*SIN(A22)*B22</f>
@@ -6854,7 +6851,7 @@
       </c>
       <c r="C23">
         <f t="shared" ref="C23:C24" si="7">O$5 + 1.5*L$5*COS(A23)*B23</f>
-        <v>635.77196130707318</v>
+        <v>571.48624702135885</v>
       </c>
       <c r="D23">
         <f t="shared" ref="D23:D24" si="8">O$6+1.5*L$6*SIN(A23)*B23</f>
@@ -6872,7 +6869,7 @@
       </c>
       <c r="C24">
         <f t="shared" si="7"/>
-        <v>678.88633485434855</v>
+        <v>614.60062056863421</v>
       </c>
       <c r="D24">
         <f t="shared" si="8"/>
@@ -6890,7 +6887,7 @@
       </c>
       <c r="C25">
         <f>O$5 + 1.5*L$5*COS(A25)*B25</f>
-        <v>771.42857142857156</v>
+        <v>707.14285714285711</v>
       </c>
       <c r="D25">
         <f>O$6+1.5*L$6*SIN(A25)*B25</f>
@@ -6908,7 +6905,7 @@
       </c>
       <c r="C26">
         <f t="shared" ref="C26:C36" si="11">O$5 + 1.5*L$5*COS(A26)*B26</f>
-        <v>739.94980162895308</v>
+        <v>675.66408734323875</v>
       </c>
       <c r="D26">
         <f t="shared" ref="D26:D36" si="12">O$6+1.5*L$6*SIN(A26)*B26</f>
@@ -6926,7 +6923,7 @@
       </c>
       <c r="C27">
         <f t="shared" si="11"/>
-        <v>653.2205929375217</v>
+        <v>588.93487865180737</v>
       </c>
       <c r="D27">
         <f t="shared" si="12"/>
@@ -6944,7 +6941,7 @@
       </c>
       <c r="C28">
         <f t="shared" si="11"/>
-        <v>532.47528042883789</v>
+        <v>468.18956614312361</v>
       </c>
       <c r="D28">
         <f t="shared" si="12"/>
@@ -6962,7 +6959,7 @@
       </c>
       <c r="C29">
         <f t="shared" si="11"/>
-        <v>407.27652774502053</v>
+        <v>342.9908134593062</v>
       </c>
       <c r="D29">
         <f t="shared" si="12"/>
@@ -6980,7 +6977,7 @@
       </c>
       <c r="C30">
         <f t="shared" si="11"/>
-        <v>308.27735600221706</v>
+        <v>243.99164171650273</v>
       </c>
       <c r="D30">
         <f t="shared" si="12"/>
@@ -6998,7 +6995,7 @@
       </c>
       <c r="C31">
         <f t="shared" si="11"/>
-        <v>259.71621515988545</v>
+        <v>195.43050087417114</v>
       </c>
       <c r="D31">
         <f t="shared" si="12"/>
@@ -7016,7 +7013,7 @@
       </c>
       <c r="C32">
         <f t="shared" si="11"/>
-        <v>273.4825661252238</v>
+        <v>209.19685183950946</v>
       </c>
       <c r="D32">
         <f t="shared" si="12"/>
@@ -7034,7 +7031,7 @@
       </c>
       <c r="C33">
         <f t="shared" si="11"/>
-        <v>346.20592606364266</v>
+        <v>281.92021177792833</v>
       </c>
       <c r="D33">
         <f t="shared" si="12"/>
@@ -7052,7 +7049,7 @@
       </c>
       <c r="C34">
         <f t="shared" si="11"/>
-        <v>460.08108014637099</v>
+        <v>395.79536586065666</v>
       </c>
       <c r="D34">
         <f t="shared" si="12"/>
@@ -7070,7 +7067,7 @@
       </c>
       <c r="C35">
         <f t="shared" si="11"/>
-        <v>587.22741911911544</v>
+        <v>522.94170483340099</v>
       </c>
       <c r="D35">
         <f t="shared" si="12"/>
@@ -7088,7 +7085,7 @@
       </c>
       <c r="C36">
         <f t="shared" si="11"/>
-        <v>696.51508481775261</v>
+        <v>632.22937053203827</v>
       </c>
       <c r="D36">
         <f t="shared" si="12"/>
@@ -7106,7 +7103,7 @@
       </c>
       <c r="C37">
         <f>O$5 + 1.5*L$5*COS(A37)*B37</f>
-        <v>761.18664513866565</v>
+        <v>696.90093085295121</v>
       </c>
       <c r="D37">
         <f>O$6+1.5*L$6*SIN(A37)*B37</f>
@@ -7124,7 +7121,7 @@
       </c>
       <c r="C38">
         <f t="shared" ref="C38:C50" si="15">O$5 + 1.5*L$5*COS(A38)*B38</f>
-        <v>857.14285714285722</v>
+        <v>792.85714285714289</v>
       </c>
       <c r="D38">
         <f t="shared" ref="D38:D50" si="16">O$6+1.5*L$6*SIN(A38)*B38</f>
@@ -7142,7 +7139,7 @@
       </c>
       <c r="C39">
         <f t="shared" si="15"/>
-        <v>815.17116407669937</v>
+        <v>750.88544979098492</v>
       </c>
       <c r="D39">
         <f t="shared" si="16"/>
@@ -7160,7 +7157,7 @@
       </c>
       <c r="C40">
         <f t="shared" si="15"/>
-        <v>699.53221915479082</v>
+        <v>635.24650486907649</v>
       </c>
       <c r="D40">
         <f t="shared" si="16"/>
@@ -7178,7 +7175,7 @@
       </c>
       <c r="C41">
         <f t="shared" si="15"/>
-        <v>538.53846914321252</v>
+        <v>474.25275485749813</v>
       </c>
       <c r="D41">
         <f t="shared" si="16"/>
@@ -7196,7 +7193,7 @@
       </c>
       <c r="C42">
         <f t="shared" si="15"/>
-        <v>371.60679889812263</v>
+        <v>307.3210846124083</v>
       </c>
       <c r="D42">
         <f t="shared" si="16"/>
@@ -7214,7 +7211,7 @@
       </c>
       <c r="C43">
         <f t="shared" si="15"/>
-        <v>239.6079032410513</v>
+        <v>175.32218895533697</v>
       </c>
       <c r="D43">
         <f t="shared" si="16"/>
@@ -7232,7 +7229,7 @@
       </c>
       <c r="C44">
         <f t="shared" si="15"/>
-        <v>174.85971545127586</v>
+        <v>110.57400116556153</v>
       </c>
       <c r="D44">
         <f t="shared" si="16"/>
@@ -7250,7 +7247,7 @@
       </c>
       <c r="C45">
         <f t="shared" si="15"/>
-        <v>193.21485007172697</v>
+        <v>128.92913578601264</v>
       </c>
       <c r="D45">
         <f t="shared" si="16"/>
@@ -7268,7 +7265,7 @@
       </c>
       <c r="C46">
         <f t="shared" si="15"/>
-        <v>290.17932998961879</v>
+        <v>225.89361570390446</v>
       </c>
       <c r="D46">
         <f t="shared" si="16"/>
@@ -7286,7 +7283,7 @@
       </c>
       <c r="C47">
         <f t="shared" si="15"/>
-        <v>442.01286876658986</v>
+        <v>377.72715448087553</v>
       </c>
       <c r="D47">
         <f t="shared" si="16"/>
@@ -7304,7 +7301,7 @@
       </c>
       <c r="C48">
         <f t="shared" si="15"/>
-        <v>611.54132073024903</v>
+        <v>547.25560644453469</v>
       </c>
       <c r="D48">
         <f t="shared" si="16"/>
@@ -7322,7 +7319,7 @@
       </c>
       <c r="C49">
         <f t="shared" si="15"/>
-        <v>757.25820832843203</v>
+        <v>692.9724940427177</v>
       </c>
       <c r="D49">
         <f t="shared" si="16"/>
@@ -7340,7 +7337,7 @@
       </c>
       <c r="C50">
         <f t="shared" si="15"/>
-        <v>843.48695542298265</v>
+        <v>779.20124113726843</v>
       </c>
       <c r="D50">
         <f t="shared" si="16"/>

</xml_diff>

<commit_message>
Removed monsters and Zero to not be able go through eachother
Till better sollution is found monsters can go through eachother and through Zero;
the ToDo file has been added in the project  files
</commit_message>
<xml_diff>
--- a/calcs.xlsx
+++ b/calcs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8136" firstSheet="7" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="3876" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="frames" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="firing accuracy" sheetId="13" r:id="rId12"/>
     <sheet name="balance game consts" sheetId="14" r:id="rId13"/>
     <sheet name="objs speed" sheetId="15" r:id="rId14"/>
+    <sheet name="twoObjsColide" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="212">
   <si>
     <t>y \ x</t>
   </si>
@@ -735,17 +736,97 @@
   <si>
     <t>divider</t>
   </si>
+  <si>
+    <t>Zero</t>
+  </si>
+  <si>
+    <t>--== Case 2 ==--</t>
+  </si>
+  <si>
+    <t>Monster</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>Monster before</t>
+  </si>
+  <si>
+    <t>Monster after</t>
+  </si>
+  <si>
+    <t>◢</t>
+  </si>
+  <si>
+    <t>{x=426.99997520446777 y=558.00000000000000 w=57.000000000000000 ...}</t>
+  </si>
+  <si>
+    <t>Rectangle</t>
+  </si>
+  <si>
+    <t>{x=382.14284181594849 y=517.57142859697342 w=57.000000000000000 ...}</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>xw1</t>
+  </si>
+  <si>
+    <t>xw2</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>y2</t>
+  </si>
+  <si>
+    <t>yh1</t>
+  </si>
+  <si>
+    <t>yh2</t>
+  </si>
+  <si>
+    <t>(yh1 &lt; y2) || (y1 &gt; yh2)</t>
+  </si>
+  <si>
+    <t>(xw1 &lt; x2) || (x1 &gt; xw2)</t>
+  </si>
+  <si>
+    <t>returns</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -795,6 +876,15 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -868,7 +958,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -986,12 +1076,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1009,16 +1147,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1029,30 +1167,49 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="10" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1200,11 +1357,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="265452928"/>
-        <c:axId val="265753728"/>
+        <c:axId val="333476992"/>
+        <c:axId val="333478528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="265452928"/>
+        <c:axId val="333476992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="800"/>
@@ -1215,13 +1372,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265753728"/>
+        <c:crossAx val="333478528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="265753728"/>
+        <c:axId val="333478528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1232,7 +1389,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265452928"/>
+        <c:crossAx val="333476992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1558,11 +1715,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="266369664"/>
-        <c:axId val="266371456"/>
+        <c:axId val="347091328"/>
+        <c:axId val="347092864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="266369664"/>
+        <c:axId val="347091328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1573,13 +1730,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266371456"/>
+        <c:crossAx val="347092864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="114"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="266371456"/>
+        <c:axId val="347092864"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1590,7 +1747,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266369664"/>
+        <c:crossAx val="347091328"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="85"/>
@@ -1828,11 +1985,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="266635136"/>
-        <c:axId val="266636672"/>
+        <c:axId val="362241408"/>
+        <c:axId val="362251392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="266635136"/>
+        <c:axId val="362241408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1842,12 +1999,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266636672"/>
+        <c:crossAx val="362251392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="266636672"/>
+        <c:axId val="362251392"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1858,13 +2015,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266635136"/>
+        <c:crossAx val="362241408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1896,6 +2054,278 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'process collisions 2'!$D$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Zero</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'process collisions 2'!$A$37:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>426.99997520446698</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>426.99997520446698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>483.99997520446698</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>483.99997520446698</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>426.99997520446698</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'process collisions 2'!$B$37:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>558</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>558</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>558</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'process collisions 2'!$D$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Monster after</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'process collisions 2'!$A$30:$A$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>382.14284181594797</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>382.14284181594797</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>439.14284181594797</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>439.14284181594797</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>382.14284181594797</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'process collisions 2'!$B$30:$B$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>557</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>557</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>515</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'process collisions 2'!$D$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Monster before</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'process collisions 2'!$A$23:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>382.14284181594797</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>382.14284181594797</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>439.14284181594797</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>439.14284181594797</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>382.14284181594797</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'process collisions 2'!$B$23:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>517.57142859697296</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>559.57142859697296</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>559.57142859697296</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>517.57142859697296</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>517.57142859697296</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="192616704"/>
+        <c:axId val="286167808"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="192616704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="286167808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="286167808"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="192616704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
@@ -1943,11 +2373,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="266542464"/>
-        <c:axId val="266552448"/>
+        <c:axId val="362284160"/>
+        <c:axId val="362285696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="266542464"/>
+        <c:axId val="362284160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1956,7 +2386,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266552448"/>
+        <c:crossAx val="362285696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1964,7 +2394,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="266552448"/>
+        <c:axId val="362285696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1975,7 +2405,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266542464"/>
+        <c:crossAx val="362284160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1996,7 +2426,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2078,11 +2508,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="266803840"/>
-        <c:axId val="266817920"/>
+        <c:axId val="362334848"/>
+        <c:axId val="362344832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="266803840"/>
+        <c:axId val="362334848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2092,12 +2522,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266817920"/>
+        <c:crossAx val="362344832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="266817920"/>
+        <c:axId val="362344832"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2108,13 +2538,221 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="266803840"/>
+        <c:crossAx val="362334848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>twoObjsColide!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Zero</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>twoObjsColide!$F$3:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>426.99997520446698</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>426.99997520446698</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>483.99997520446698</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>483.99997520446698</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>426.99997520446698</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>twoObjsColide!$G$3:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>558</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>558</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>558</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>twoObjsColide!$F$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Monster</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>twoObjsColide!$F$9:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>382.14284181594797</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>382.14284181594797</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>439.14284181594797</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>439.14284181594797</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>382.14284181594797</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>twoObjsColide!$G$9:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>517.57142859697296</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>559.57142859697296</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>559.57142859697296</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>517.57142859697296</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>517.57142859697296</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="164247424"/>
+        <c:axId val="164245888"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="164247424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="164245888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="164245888"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="164247424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2884,16 +3522,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>148590</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>365760</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>148590</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2907,6 +3545,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2964,6 +3634,41 @@
       <xdr:colOff>144780</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3240,7 +3945,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3892,7 +4597,7 @@
       </c>
       <c r="B4">
         <f ca="1">RANDBETWEEN(0,B3)</f>
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3901,7 +4606,7 @@
       </c>
       <c r="B5">
         <f ca="1">B4-B3/2</f>
-        <v>-10</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
         <v>164</v>
@@ -4449,6 +5154,431 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="37"/>
+      <c r="B1" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="F2" s="42" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="39"/>
+      <c r="B3" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="40">
+        <v>426.99997520446698</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="F3">
+        <f>C3</f>
+        <v>426.99997520446698</v>
+      </c>
+      <c r="G3">
+        <f>C4</f>
+        <v>558</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="39"/>
+      <c r="B4" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="40">
+        <v>558</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="F4">
+        <f>C3</f>
+        <v>426.99997520446698</v>
+      </c>
+      <c r="G4">
+        <f>C4+C6</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="39"/>
+      <c r="B5" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="40">
+        <v>57</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="F5">
+        <f>C3+C5</f>
+        <v>483.99997520446698</v>
+      </c>
+      <c r="G5">
+        <f>C4+C6</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="39"/>
+      <c r="B6" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="40">
+        <v>42</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="F6">
+        <f>C3+C5</f>
+        <v>483.99997520446698</v>
+      </c>
+      <c r="G6">
+        <f>C4</f>
+        <v>558</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="37"/>
+      <c r="B7" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="F7">
+        <f>C3</f>
+        <v>426.99997520446698</v>
+      </c>
+      <c r="G7">
+        <f>C4</f>
+        <v>558</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="39" t="s">
+        <v>197</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="F8" s="42" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="39"/>
+      <c r="B9" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="40">
+        <v>382.14284181594797</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="F9">
+        <f>C9</f>
+        <v>382.14284181594797</v>
+      </c>
+      <c r="G9">
+        <f>C10</f>
+        <v>517.57142859697296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="39"/>
+      <c r="B10" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="40">
+        <v>517.57142859697296</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="F10">
+        <f>C9</f>
+        <v>382.14284181594797</v>
+      </c>
+      <c r="G10">
+        <f>C10+C12</f>
+        <v>559.57142859697296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="39"/>
+      <c r="B11" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="40">
+        <v>57</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="F11">
+        <f>C9+C11</f>
+        <v>439.14284181594797</v>
+      </c>
+      <c r="G11">
+        <f>C10+C12</f>
+        <v>559.57142859697296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="39"/>
+      <c r="B12" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="40">
+        <v>42</v>
+      </c>
+      <c r="D12" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="F12">
+        <f>C9+C11</f>
+        <v>439.14284181594797</v>
+      </c>
+      <c r="G12">
+        <f>C10</f>
+        <v>517.57142859697296</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="37"/>
+      <c r="B13" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="F13">
+        <f>C9</f>
+        <v>382.14284181594797</v>
+      </c>
+      <c r="G13">
+        <f>C10</f>
+        <v>517.57142859697296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="39"/>
+      <c r="B14" s="40" t="s">
+        <v>201</v>
+      </c>
+      <c r="C14" s="40">
+        <v>426.99997520446698</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="39"/>
+      <c r="B15" s="40" t="s">
+        <v>205</v>
+      </c>
+      <c r="C15" s="40">
+        <v>558</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="39"/>
+      <c r="B16" s="40" t="s">
+        <v>203</v>
+      </c>
+      <c r="C16" s="40">
+        <v>483.99997520446698</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="39"/>
+      <c r="B17" s="40" t="s">
+        <v>207</v>
+      </c>
+      <c r="C17" s="40">
+        <v>600</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="39"/>
+      <c r="B18" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="C18" s="40">
+        <v>382.14284181594797</v>
+      </c>
+      <c r="D18" s="40" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="39"/>
+      <c r="B19" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="C19" s="40">
+        <v>517.57142859697296</v>
+      </c>
+      <c r="D19" s="40" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="39"/>
+      <c r="B20" s="40" t="s">
+        <v>204</v>
+      </c>
+      <c r="C20" s="40">
+        <v>439.14284181594797</v>
+      </c>
+      <c r="D20" s="40" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="39"/>
+      <c r="B21" s="40" t="s">
+        <v>208</v>
+      </c>
+      <c r="C21" s="40">
+        <v>559.57142859697296</v>
+      </c>
+      <c r="D21" s="40" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" t="b">
+        <f>C17 &lt; C19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" t="b">
+        <f>C15 &gt; C21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>209</v>
+      </c>
+      <c r="C25" t="b">
+        <f>OR(C23,C24)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" t="b">
+        <f>C16 &lt; C18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" t="b">
+        <f>C14 &gt; C20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>210</v>
+      </c>
+      <c r="C28" t="b">
+        <f>OR(C26,C27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>211</v>
+      </c>
+      <c r="C29" t="b">
+        <f>NOT(OR(C25,C28))</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6366,7 +7496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -7353,10 +8483,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7610,8 +8740,252 @@
         <v>510</v>
       </c>
     </row>
+    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:5" s="32" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="36" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f>E23</f>
+        <v>382.14284181594797</v>
+      </c>
+      <c r="B23">
+        <f>E24</f>
+        <v>517.57142859697296</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <v>382.14284181594797</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f>E23</f>
+        <v>382.14284181594797</v>
+      </c>
+      <c r="B24">
+        <f>E24+E26</f>
+        <v>559.57142859697296</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24">
+        <v>517.57142859697296</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f>E23+E25</f>
+        <v>439.14284181594797</v>
+      </c>
+      <c r="B25">
+        <f>E24+E26</f>
+        <v>559.57142859697296</v>
+      </c>
+      <c r="D25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f>E23+E25</f>
+        <v>439.14284181594797</v>
+      </c>
+      <c r="B26">
+        <f>E24</f>
+        <v>517.57142859697296</v>
+      </c>
+      <c r="D26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <f>E23</f>
+        <v>382.14284181594797</v>
+      </c>
+      <c r="B27">
+        <f>E24</f>
+        <v>517.57142859697296</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f>E30</f>
+        <v>382.14284181594797</v>
+      </c>
+      <c r="B30">
+        <f>E31</f>
+        <v>515</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30">
+        <v>382.14284181594797</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f>E30</f>
+        <v>382.14284181594797</v>
+      </c>
+      <c r="B31">
+        <f>E31+E33</f>
+        <v>557</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f>E30+E32</f>
+        <v>439.14284181594797</v>
+      </c>
+      <c r="B32">
+        <f>E31+E33</f>
+        <v>557</v>
+      </c>
+      <c r="D32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f>E30+E32</f>
+        <v>439.14284181594797</v>
+      </c>
+      <c r="B33">
+        <f>E31</f>
+        <v>515</v>
+      </c>
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f>E30</f>
+        <v>382.14284181594797</v>
+      </c>
+      <c r="B34">
+        <f>E31</f>
+        <v>515</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f>E37</f>
+        <v>426.99997520446698</v>
+      </c>
+      <c r="B37">
+        <f>E38</f>
+        <v>558</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37">
+        <v>426.99997520446698</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <f>E37</f>
+        <v>426.99997520446698</v>
+      </c>
+      <c r="B38">
+        <f>E38+E40</f>
+        <v>600</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <f>E37+E39</f>
+        <v>483.99997520446698</v>
+      </c>
+      <c r="B39">
+        <f>E38+E40</f>
+        <v>600</v>
+      </c>
+      <c r="D39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <f>E37+E39</f>
+        <v>483.99997520446698</v>
+      </c>
+      <c r="B40">
+        <f>E38</f>
+        <v>558</v>
+      </c>
+      <c r="D40" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <f>E37</f>
+        <v>426.99997520446698</v>
+      </c>
+      <c r="B41">
+        <f>E38</f>
+        <v>558</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add: Load game functionality finished
</commit_message>
<xml_diff>
--- a/calcs.xlsx
+++ b/calcs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="3876" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="3876" firstSheet="11" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="frames" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="twoObjsColide" sheetId="16" r:id="rId15"/>
     <sheet name="zero-monster-colide" sheetId="18" r:id="rId16"/>
     <sheet name="Timer" sheetId="19" r:id="rId17"/>
+    <sheet name="resMan objects" sheetId="20" r:id="rId18"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="255">
   <si>
     <t>y \ x</t>
   </si>
@@ -866,6 +867,78 @@
   </si>
   <si>
     <t>elapsedSeconds</t>
+  </si>
+  <si>
+    <t>ResourcesManager::loadResources()</t>
+  </si>
+  <si>
+    <t>imagesNames</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>resourcesTypes</t>
+  </si>
+  <si>
+    <t>vector&lt;OBJ_TYPE&gt;</t>
+  </si>
+  <si>
+    <t>UMAP&lt;OBJ_TYPE, string&gt;</t>
+  </si>
+  <si>
+    <t>soundNames</t>
+  </si>
+  <si>
+    <t>UMAP&lt;OBJ_TYPE, std::vector&lt;std::string&gt; &gt;</t>
+  </si>
+  <si>
+    <t>soundsRanges</t>
+  </si>
+  <si>
+    <t>UMAP&lt;OBJ_TYPE, std::vector&lt;size_t&gt; &gt;</t>
+  </si>
+  <si>
+    <t>musicBackgroundNames</t>
+  </si>
+  <si>
+    <t>UMAP&lt;OBJ_TYPE, std::pair&lt;std::string, sf::Texture&gt;&gt;</t>
+  </si>
+  <si>
+    <t>m_textures</t>
+  </si>
+  <si>
+    <t>^---      resType,              pair(loadPath,   texture)</t>
+  </si>
+  <si>
+    <t>for (auto&amp; typeSoundsNames : soundNames)</t>
+  </si>
+  <si>
+    <t>typeSoundsNames</t>
+  </si>
+  <si>
+    <t>pair&lt;OBJ_TYPE, std::vector&lt;std::string&gt; &gt;</t>
+  </si>
+  <si>
+    <t>^---  resType,             vector(soundFilePaths)</t>
+  </si>
+  <si>
+    <t>m_soundBuffers</t>
+  </si>
+  <si>
+    <t>UMAP&lt;OBJ_TYPE, SoundBuffersHolder &gt;</t>
+  </si>
+  <si>
+    <t>for (auto&amp; typeSoundsRanges : soundsRanges)</t>
+  </si>
+  <si>
+    <t>typeSoundsRanges</t>
+  </si>
+  <si>
+    <t>pair&lt;OBJ_TYPE, std::vector&lt;size_t&gt; &gt;</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1329,6 +1402,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -1482,11 +1558,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="214275584"/>
-        <c:axId val="214277120"/>
+        <c:axId val="229547008"/>
+        <c:axId val="229569280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="214275584"/>
+        <c:axId val="229547008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="800"/>
@@ -1497,13 +1573,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214277120"/>
+        <c:crossAx val="229569280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="214277120"/>
+        <c:axId val="229569280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1514,7 +1590,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214275584"/>
+        <c:crossAx val="229547008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1839,11 +1915,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="235156224"/>
-        <c:axId val="235157760"/>
+        <c:axId val="229980416"/>
+        <c:axId val="229994496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="235156224"/>
+        <c:axId val="229980416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1854,13 +1930,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235157760"/>
+        <c:crossAx val="229994496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="114"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="235157760"/>
+        <c:axId val="229994496"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1871,7 +1947,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235156224"/>
+        <c:crossAx val="229980416"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="85"/>
@@ -2109,11 +2185,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="235769856"/>
-        <c:axId val="235771392"/>
+        <c:axId val="230180352"/>
+        <c:axId val="230181888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="235769856"/>
+        <c:axId val="230180352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2123,12 +2199,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235771392"/>
+        <c:crossAx val="230181888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="235771392"/>
+        <c:axId val="230181888"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2139,7 +2215,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235769856"/>
+        <c:crossAx val="230180352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2380,11 +2456,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="235670144"/>
-        <c:axId val="235671936"/>
+        <c:axId val="230213504"/>
+        <c:axId val="230215040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="235670144"/>
+        <c:axId val="230213504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2394,12 +2470,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235671936"/>
+        <c:crossAx val="230215040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="235671936"/>
+        <c:axId val="230215040"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2410,7 +2486,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235670144"/>
+        <c:crossAx val="230213504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2495,11 +2571,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="235698048"/>
-        <c:axId val="235699584"/>
+        <c:axId val="234934272"/>
+        <c:axId val="234935808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="235698048"/>
+        <c:axId val="234934272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2508,7 +2584,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235699584"/>
+        <c:crossAx val="234935808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2516,7 +2592,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235699584"/>
+        <c:axId val="234935808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2527,7 +2603,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235698048"/>
+        <c:crossAx val="234934272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2630,11 +2706,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="235715968"/>
-        <c:axId val="235816064"/>
+        <c:axId val="235345408"/>
+        <c:axId val="235346944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="235715968"/>
+        <c:axId val="235345408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2644,12 +2720,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235816064"/>
+        <c:crossAx val="235346944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="235816064"/>
+        <c:axId val="235346944"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2660,7 +2736,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235715968"/>
+        <c:crossAx val="235345408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2837,11 +2913,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="235496192"/>
-        <c:axId val="235497728"/>
+        <c:axId val="235553152"/>
+        <c:axId val="235554688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="235496192"/>
+        <c:axId val="235553152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2851,12 +2927,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235497728"/>
+        <c:crossAx val="235554688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="235497728"/>
+        <c:axId val="235554688"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2867,7 +2943,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235496192"/>
+        <c:crossAx val="235553152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3054,11 +3130,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="235084800"/>
-        <c:axId val="235086592"/>
+        <c:axId val="229894784"/>
+        <c:axId val="229896576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="235084800"/>
+        <c:axId val="229894784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3068,12 +3144,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235086592"/>
+        <c:crossAx val="229896576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="235086592"/>
+        <c:axId val="229896576"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3084,7 +3160,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235084800"/>
+        <c:crossAx val="229894784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4330,7 +4406,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4982,7 +5058,7 @@
       </c>
       <c r="B4">
         <f ca="1">RANDBETWEEN(0,B3)</f>
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -4991,7 +5067,7 @@
       </c>
       <c r="B5">
         <f ca="1">B4-B3/2</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D5" t="s">
         <v>164</v>
@@ -6684,6 +6760,135 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="60" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="60"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>242</v>
+      </c>
+      <c r="B7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>244</v>
+      </c>
+      <c r="B9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>247</v>
+      </c>
+      <c r="B13" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>250</v>
+      </c>
+      <c r="B16" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>253</v>
+      </c>
+      <c r="B19" t="s">
+        <v>254</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
@@ -6831,7 +7036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>

</xml_diff>